<commit_message>
removed external links from template and confirmed save issue resolved in add-in
</commit_message>
<xml_diff>
--- a/ScrumTeamStats_Template.xlsx
+++ b/ScrumTeamStats_Template.xlsx
@@ -8,19 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Git/vba-jira/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3E7104-809C-6349-9667-39518350D10F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94B548B-1D4D-894B-84A3-DCF209BFAE57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="28060" windowHeight="27820" xr2:uid="{29FB89B4-D308-7843-B61E-411B20763035}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="28060" windowHeight="27820" xr2:uid="{29FB89B4-D308-7843-B61E-411B20763035}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Metrics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Team Metrics'!$B$2:$AP$42</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,30 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="79">
   <si>
     <t>Feature</t>
   </si>
@@ -325,6 +297,9 @@
   </si>
   <si>
     <t>Number of work items delivered. Latest versus 3 month avg.</t>
+  </si>
+  <si>
+    <t>Amount of time remaining from the burndown at the end of the most recent sprint (CMS 20.01). The total Active Time for the same period was: 5w 4d 5h</t>
   </si>
 </sst>
 </file>
@@ -1062,6 +1037,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="19" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="19" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="19" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1080,143 +1103,20 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1231,10 +1131,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -1287,62 +1205,119 @@
     <xf numFmtId="168" fontId="9" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="19" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="19" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="19" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7076,22 +7051,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="jiratime"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7396,7 +7355,7 @@
   <dimension ref="B2:BN51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+      <selection activeCell="S49" sqref="S49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7406,8 +7365,8 @@
     <col min="42" max="42" width="2.6640625" style="1" customWidth="1"/>
     <col min="43" max="43" width="6" style="1" customWidth="1"/>
     <col min="44" max="44" width="6" style="50" customWidth="1"/>
-    <col min="45" max="45" width="10.5" style="133" bestFit="1" customWidth="1"/>
-    <col min="46" max="61" width="6" style="133" customWidth="1"/>
+    <col min="45" max="45" width="10.5" style="51" bestFit="1" customWidth="1"/>
+    <col min="46" max="61" width="6" style="51" customWidth="1"/>
     <col min="62" max="64" width="6" style="50" customWidth="1"/>
     <col min="65" max="65" width="4" style="50" customWidth="1"/>
     <col min="66" max="66" width="3.6640625" style="50" customWidth="1"/>
@@ -7442,284 +7401,283 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
-      <c r="AE2" s="58"/>
-      <c r="AF2" s="58"/>
-      <c r="AG2" s="58"/>
-      <c r="AH2" s="58"/>
-      <c r="AI2" s="58"/>
-      <c r="AJ2" s="58"/>
-      <c r="AK2" s="58"/>
-      <c r="AL2" s="58"/>
-      <c r="AM2" s="58"/>
-      <c r="AN2" s="58"/>
-      <c r="AO2" s="58"/>
-      <c r="AP2" s="59"/>
-      <c r="AT2" s="134" t="s">
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
+      <c r="O2" s="144"/>
+      <c r="P2" s="144"/>
+      <c r="Q2" s="144"/>
+      <c r="R2" s="144"/>
+      <c r="S2" s="144"/>
+      <c r="T2" s="144"/>
+      <c r="U2" s="144"/>
+      <c r="V2" s="144"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Y2" s="144"/>
+      <c r="Z2" s="144"/>
+      <c r="AA2" s="144"/>
+      <c r="AB2" s="144"/>
+      <c r="AC2" s="144"/>
+      <c r="AD2" s="144"/>
+      <c r="AE2" s="144"/>
+      <c r="AF2" s="144"/>
+      <c r="AG2" s="144"/>
+      <c r="AH2" s="144"/>
+      <c r="AI2" s="144"/>
+      <c r="AJ2" s="144"/>
+      <c r="AK2" s="144"/>
+      <c r="AL2" s="144"/>
+      <c r="AM2" s="144"/>
+      <c r="AN2" s="144"/>
+      <c r="AO2" s="144"/>
+      <c r="AP2" s="145"/>
+      <c r="AT2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="AU2" s="134" t="s">
+      <c r="AU2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="AV2" s="134" t="s">
+      <c r="AV2" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="AW2" s="134" t="s">
+      <c r="AW2" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="AX2" s="134"/>
+      <c r="AX2" s="92"/>
     </row>
     <row r="3" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="61"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="61"/>
-      <c r="AG3" s="61"/>
-      <c r="AH3" s="61"/>
-      <c r="AI3" s="61"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="61"/>
-      <c r="AL3" s="61"/>
-      <c r="AM3" s="61"/>
-      <c r="AN3" s="61"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="62"/>
-      <c r="AS3" s="135" t="s">
+      <c r="B3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="147"/>
+      <c r="M3" s="147"/>
+      <c r="N3" s="147"/>
+      <c r="O3" s="147"/>
+      <c r="P3" s="147"/>
+      <c r="Q3" s="147"/>
+      <c r="R3" s="147"/>
+      <c r="S3" s="147"/>
+      <c r="T3" s="147"/>
+      <c r="U3" s="147"/>
+      <c r="V3" s="147"/>
+      <c r="W3" s="147"/>
+      <c r="X3" s="147"/>
+      <c r="Y3" s="147"/>
+      <c r="Z3" s="147"/>
+      <c r="AA3" s="147"/>
+      <c r="AB3" s="147"/>
+      <c r="AC3" s="147"/>
+      <c r="AD3" s="147"/>
+      <c r="AE3" s="147"/>
+      <c r="AF3" s="147"/>
+      <c r="AG3" s="147"/>
+      <c r="AH3" s="147"/>
+      <c r="AI3" s="147"/>
+      <c r="AJ3" s="147"/>
+      <c r="AK3" s="147"/>
+      <c r="AL3" s="147"/>
+      <c r="AM3" s="147"/>
+      <c r="AN3" s="147"/>
+      <c r="AO3" s="147"/>
+      <c r="AP3" s="148"/>
+      <c r="AS3" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="AT3" s="134"/>
-      <c r="AU3" s="134"/>
-      <c r="AV3" s="134"/>
-      <c r="AW3" s="134"/>
-      <c r="AX3" s="134"/>
+      <c r="AT3" s="92"/>
+      <c r="AU3" s="92"/>
+      <c r="AV3" s="92"/>
+      <c r="AW3" s="92"/>
+      <c r="AX3" s="92"/>
     </row>
     <row r="4" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="AP4" s="3"/>
-      <c r="AS4" s="135">
+      <c r="AS4" s="52">
         <v>43992</v>
       </c>
-      <c r="AT4" s="134"/>
-      <c r="AU4" s="134"/>
-      <c r="AV4" s="134"/>
-      <c r="AW4" s="134"/>
-      <c r="AX4" s="134"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="92"/>
     </row>
     <row r="5" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="99">
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="140">
         <f>BB22</f>
         <v>0.88</v>
       </c>
-      <c r="K5" s="99"/>
-      <c r="L5" s="70" t="s">
+      <c r="K5" s="140"/>
+      <c r="L5" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="71"/>
-      <c r="X5" s="89" t="s">
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="124"/>
+      <c r="Q5" s="124"/>
+      <c r="R5" s="124"/>
+      <c r="S5" s="124"/>
+      <c r="T5" s="125"/>
+      <c r="X5" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="82"/>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="51"/>
-      <c r="AC5" s="52"/>
-      <c r="AD5" s="67" t="s">
+      <c r="Y5" s="116"/>
+      <c r="Z5" s="116"/>
+      <c r="AA5" s="116"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="AE5" s="67"/>
-      <c r="AF5" s="70" t="str" cm="1">
-        <f t="array" ref="AF5" xml:space="preserve"> "Amount of time remaining from the burndown at the end of the most recent sprint (" &amp; AS3 &amp; "). The total Active Time for the same period was: " &amp; [1]!jiratime(BB42)</f>
-        <v>Amount of time remaining from the burndown at the end of the most recent sprint (CMS 20.01). The total Active Time for the same period was: 5w 4d 5h</v>
-      </c>
-      <c r="AG5" s="70"/>
-      <c r="AH5" s="70"/>
-      <c r="AI5" s="70"/>
-      <c r="AJ5" s="70"/>
-      <c r="AK5" s="70"/>
-      <c r="AL5" s="70"/>
-      <c r="AM5" s="70"/>
-      <c r="AN5" s="71"/>
+      <c r="AE5" s="121"/>
+      <c r="AF5" s="124" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG5" s="124"/>
+      <c r="AH5" s="124"/>
+      <c r="AI5" s="124"/>
+      <c r="AJ5" s="124"/>
+      <c r="AK5" s="124"/>
+      <c r="AL5" s="124"/>
+      <c r="AM5" s="124"/>
+      <c r="AN5" s="125"/>
       <c r="AP5" s="3"/>
-      <c r="AS5" s="133" t="s">
+      <c r="AS5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="AT5" s="136">
+      <c r="AT5" s="53">
         <v>5</v>
       </c>
-      <c r="AU5" s="136">
+      <c r="AU5" s="53">
         <v>3</v>
       </c>
-      <c r="AV5" s="136">
+      <c r="AV5" s="53">
         <v>6</v>
       </c>
-      <c r="AW5" s="136">
+      <c r="AW5" s="53">
         <v>2</v>
       </c>
-      <c r="AX5" s="136"/>
+      <c r="AX5" s="53"/>
     </row>
     <row r="6" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="73"/>
-      <c r="X6" s="95"/>
-      <c r="Y6" s="96"/>
-      <c r="Z6" s="96"/>
-      <c r="AA6" s="96"/>
-      <c r="AB6" s="53"/>
-      <c r="AC6" s="54"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="68"/>
-      <c r="AF6" s="72"/>
-      <c r="AG6" s="72"/>
-      <c r="AH6" s="72"/>
-      <c r="AI6" s="72"/>
-      <c r="AJ6" s="72"/>
-      <c r="AK6" s="72"/>
-      <c r="AL6" s="72"/>
-      <c r="AM6" s="72"/>
-      <c r="AN6" s="73"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="137"/>
+      <c r="F6" s="137"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="63"/>
+      <c r="X6" s="136"/>
+      <c r="Y6" s="137"/>
+      <c r="Z6" s="137"/>
+      <c r="AA6" s="137"/>
+      <c r="AB6" s="73"/>
+      <c r="AC6" s="74"/>
+      <c r="AD6" s="122"/>
+      <c r="AE6" s="122"/>
+      <c r="AF6" s="62"/>
+      <c r="AG6" s="62"/>
+      <c r="AH6" s="62"/>
+      <c r="AI6" s="62"/>
+      <c r="AJ6" s="62"/>
+      <c r="AK6" s="62"/>
+      <c r="AL6" s="62"/>
+      <c r="AM6" s="62"/>
+      <c r="AN6" s="63"/>
       <c r="AP6" s="3"/>
-      <c r="AS6" s="133" t="s">
+      <c r="AS6" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="AT6" s="136">
+      <c r="AT6" s="53">
         <v>7</v>
       </c>
-      <c r="AU6" s="136">
+      <c r="AU6" s="53">
         <v>1</v>
       </c>
-      <c r="AV6" s="136">
+      <c r="AV6" s="53">
         <v>1.6666666666666667</v>
       </c>
-      <c r="AW6" s="136">
+      <c r="AW6" s="53">
         <v>1.3333333333333333</v>
       </c>
-      <c r="AX6" s="136"/>
+      <c r="AX6" s="53"/>
     </row>
     <row r="7" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="75"/>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="98"/>
-      <c r="Z7" s="98"/>
-      <c r="AA7" s="98"/>
-      <c r="AB7" s="55"/>
-      <c r="AC7" s="56"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="74"/>
-      <c r="AG7" s="74"/>
-      <c r="AH7" s="74"/>
-      <c r="AI7" s="74"/>
-      <c r="AJ7" s="74"/>
-      <c r="AK7" s="74"/>
-      <c r="AL7" s="74"/>
-      <c r="AM7" s="74"/>
-      <c r="AN7" s="75"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="66"/>
+      <c r="X7" s="138"/>
+      <c r="Y7" s="139"/>
+      <c r="Z7" s="139"/>
+      <c r="AA7" s="139"/>
+      <c r="AB7" s="75"/>
+      <c r="AC7" s="76"/>
+      <c r="AD7" s="123"/>
+      <c r="AE7" s="123"/>
+      <c r="AF7" s="65"/>
+      <c r="AG7" s="65"/>
+      <c r="AH7" s="65"/>
+      <c r="AI7" s="65"/>
+      <c r="AJ7" s="65"/>
+      <c r="AK7" s="65"/>
+      <c r="AL7" s="65"/>
+      <c r="AM7" s="65"/>
+      <c r="AN7" s="66"/>
       <c r="AP7" s="3"/>
     </row>
     <row r="8" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7728,7 +7686,7 @@
     </row>
     <row r="9" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="126" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="4"/>
@@ -7749,7 +7707,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="5"/>
-      <c r="W9" s="79" t="s">
+      <c r="W9" s="129" t="s">
         <v>11</v>
       </c>
       <c r="X9" s="6"/>
@@ -7774,715 +7732,715 @@
     </row>
     <row r="10" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="82" t="s">
+      <c r="C10" s="127"/>
+      <c r="D10" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="85" t="s">
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="86"/>
-      <c r="M10" s="89" t="s">
+      <c r="K10" s="133"/>
+      <c r="M10" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="83"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="91">
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="117">
         <v>0.46666666666666667</v>
       </c>
-      <c r="T10" s="92"/>
+      <c r="T10" s="118"/>
       <c r="U10" s="8"/>
-      <c r="W10" s="80"/>
-      <c r="X10" s="102" t="s">
+      <c r="W10" s="130"/>
+      <c r="X10" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="Y10" s="83"/>
-      <c r="Z10" s="83"/>
-      <c r="AA10" s="83"/>
-      <c r="AB10" s="51"/>
-      <c r="AC10" s="52"/>
-      <c r="AD10" s="103">
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="71"/>
+      <c r="AC10" s="72"/>
+      <c r="AD10" s="82">
         <v>156</v>
       </c>
-      <c r="AE10" s="104"/>
-      <c r="AG10" s="89" t="s">
+      <c r="AE10" s="83"/>
+      <c r="AG10" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="AH10" s="83"/>
-      <c r="AI10" s="83"/>
-      <c r="AJ10" s="83"/>
-      <c r="AK10" s="51"/>
-      <c r="AL10" s="52"/>
-      <c r="AM10" s="63">
+      <c r="AH10" s="68"/>
+      <c r="AI10" s="68"/>
+      <c r="AJ10" s="68"/>
+      <c r="AK10" s="71"/>
+      <c r="AL10" s="72"/>
+      <c r="AM10" s="112">
         <v>3</v>
       </c>
-      <c r="AN10" s="64"/>
+      <c r="AN10" s="113"/>
       <c r="AO10" s="9"/>
       <c r="AP10" s="3"/>
     </row>
     <row r="11" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="88"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="84"/>
-      <c r="O11" s="84"/>
-      <c r="P11" s="84"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="93"/>
-      <c r="T11" s="94"/>
+      <c r="C11" s="127"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="134"/>
+      <c r="K11" s="135"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="70"/>
+      <c r="P11" s="70"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="119"/>
+      <c r="T11" s="120"/>
       <c r="U11" s="8"/>
-      <c r="W11" s="80"/>
-      <c r="X11" s="90"/>
-      <c r="Y11" s="84"/>
-      <c r="Z11" s="84"/>
-      <c r="AA11" s="84"/>
-      <c r="AB11" s="53"/>
-      <c r="AC11" s="54"/>
-      <c r="AD11" s="105"/>
-      <c r="AE11" s="106"/>
-      <c r="AG11" s="90"/>
-      <c r="AH11" s="84"/>
-      <c r="AI11" s="84"/>
-      <c r="AJ11" s="84"/>
-      <c r="AK11" s="53"/>
-      <c r="AL11" s="54"/>
-      <c r="AM11" s="65"/>
-      <c r="AN11" s="66"/>
+      <c r="W11" s="130"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="70"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="73"/>
+      <c r="AC11" s="74"/>
+      <c r="AD11" s="84"/>
+      <c r="AE11" s="85"/>
+      <c r="AG11" s="69"/>
+      <c r="AH11" s="70"/>
+      <c r="AI11" s="70"/>
+      <c r="AJ11" s="70"/>
+      <c r="AK11" s="73"/>
+      <c r="AL11" s="74"/>
+      <c r="AM11" s="114"/>
+      <c r="AN11" s="115"/>
       <c r="AO11" s="9"/>
       <c r="AP11" s="3"/>
-      <c r="AS11" s="133" t="s">
+      <c r="AS11" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="AT11" s="137">
+      <c r="AT11" s="54">
         <v>0</v>
       </c>
-      <c r="AU11" s="137">
+      <c r="AU11" s="54">
         <v>3</v>
       </c>
-      <c r="AV11" s="137">
+      <c r="AV11" s="54">
         <v>9</v>
       </c>
-      <c r="AW11" s="137">
+      <c r="AW11" s="54">
         <v>2</v>
       </c>
-      <c r="AX11" s="137">
+      <c r="AX11" s="54">
         <v>6</v>
       </c>
-      <c r="AY11" s="137">
+      <c r="AY11" s="54">
         <v>4</v>
       </c>
-      <c r="AZ11" s="137">
+      <c r="AZ11" s="54">
         <v>5</v>
       </c>
-      <c r="BA11" s="137">
+      <c r="BA11" s="54">
         <v>2</v>
       </c>
-      <c r="BB11" s="137">
+      <c r="BB11" s="54">
         <v>13</v>
       </c>
-      <c r="BC11" s="137">
+      <c r="BC11" s="54">
         <v>9</v>
       </c>
-      <c r="BD11" s="137">
+      <c r="BD11" s="54">
         <v>0</v>
       </c>
-      <c r="BE11" s="137">
+      <c r="BE11" s="54">
         <v>5</v>
       </c>
-      <c r="BF11" s="137">
+      <c r="BF11" s="54">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="88"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="84"/>
-      <c r="O12" s="84"/>
-      <c r="P12" s="84"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="93"/>
-      <c r="T12" s="94"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="134"/>
+      <c r="K12" s="135"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="70"/>
+      <c r="P12" s="70"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="76"/>
+      <c r="S12" s="119"/>
+      <c r="T12" s="120"/>
       <c r="U12" s="8"/>
-      <c r="W12" s="80"/>
-      <c r="X12" s="90"/>
-      <c r="Y12" s="84"/>
-      <c r="Z12" s="84"/>
-      <c r="AA12" s="84"/>
-      <c r="AB12" s="55"/>
-      <c r="AC12" s="56"/>
-      <c r="AD12" s="105"/>
-      <c r="AE12" s="106"/>
-      <c r="AG12" s="90"/>
-      <c r="AH12" s="84"/>
-      <c r="AI12" s="84"/>
-      <c r="AJ12" s="84"/>
-      <c r="AK12" s="55"/>
-      <c r="AL12" s="56"/>
-      <c r="AM12" s="65"/>
-      <c r="AN12" s="66"/>
+      <c r="W12" s="130"/>
+      <c r="X12" s="69"/>
+      <c r="Y12" s="70"/>
+      <c r="Z12" s="70"/>
+      <c r="AA12" s="70"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="76"/>
+      <c r="AD12" s="84"/>
+      <c r="AE12" s="85"/>
+      <c r="AG12" s="69"/>
+      <c r="AH12" s="70"/>
+      <c r="AI12" s="70"/>
+      <c r="AJ12" s="70"/>
+      <c r="AK12" s="75"/>
+      <c r="AL12" s="76"/>
+      <c r="AM12" s="114"/>
+      <c r="AN12" s="115"/>
       <c r="AO12" s="9"/>
       <c r="AP12" s="3"/>
-      <c r="AS12" s="133" t="s">
+      <c r="AS12" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AT12" s="137">
+      <c r="AT12" s="54">
         <v>1</v>
       </c>
-      <c r="AU12" s="137">
+      <c r="AU12" s="54">
         <v>1</v>
       </c>
-      <c r="AV12" s="137">
+      <c r="AV12" s="54">
         <v>3</v>
       </c>
-      <c r="AW12" s="137">
+      <c r="AW12" s="54">
         <v>1</v>
       </c>
-      <c r="AX12" s="137">
+      <c r="AX12" s="54">
         <v>1</v>
       </c>
-      <c r="AY12" s="137">
+      <c r="AY12" s="54">
         <v>2</v>
       </c>
-      <c r="AZ12" s="137">
+      <c r="AZ12" s="54">
         <v>3</v>
       </c>
-      <c r="BA12" s="137">
+      <c r="BA12" s="54">
         <v>1</v>
       </c>
-      <c r="BB12" s="137">
+      <c r="BB12" s="54">
         <v>2</v>
       </c>
-      <c r="BC12" s="137">
+      <c r="BC12" s="54">
         <v>0</v>
       </c>
-      <c r="BD12" s="137">
+      <c r="BD12" s="54">
         <v>0</v>
       </c>
-      <c r="BE12" s="137">
+      <c r="BE12" s="54">
         <v>3</v>
       </c>
-      <c r="BF12" s="137">
+      <c r="BF12" s="54">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="72" t="s">
+      <c r="C13" s="127"/>
+      <c r="D13" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="73"/>
-      <c r="M13" s="107" t="str">
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="63"/>
+      <c r="M13" s="61" t="str">
         <f xml:space="preserve"> "Completed Story Points / Committed Story Points for the most recent sprint (" &amp; AS3 &amp; ")"</f>
         <v>Completed Story Points / Committed Story Points for the most recent sprint (CMS 20.01)</v>
       </c>
-      <c r="N13" s="72"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="72"/>
-      <c r="R13" s="72"/>
-      <c r="S13" s="72"/>
-      <c r="T13" s="73"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="63"/>
       <c r="U13" s="8"/>
-      <c r="W13" s="80"/>
-      <c r="X13" s="107" t="s">
+      <c r="W13" s="130"/>
+      <c r="X13" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="Y13" s="72"/>
-      <c r="Z13" s="72"/>
-      <c r="AA13" s="72"/>
-      <c r="AB13" s="72"/>
-      <c r="AC13" s="72"/>
-      <c r="AD13" s="72"/>
-      <c r="AE13" s="73"/>
-      <c r="AG13" s="107" t="str">
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="62"/>
+      <c r="AD13" s="62"/>
+      <c r="AE13" s="63"/>
+      <c r="AG13" s="61" t="str">
         <f>"Number of code deployments in the previous calendar month ("&amp;TEXT(BE15,"mmm")&amp;")"</f>
         <v>Number of code deployments in the previous calendar month (May)</v>
       </c>
-      <c r="AH13" s="72"/>
-      <c r="AI13" s="72"/>
-      <c r="AJ13" s="72"/>
-      <c r="AK13" s="72"/>
-      <c r="AL13" s="72"/>
-      <c r="AM13" s="72"/>
-      <c r="AN13" s="73"/>
+      <c r="AH13" s="62"/>
+      <c r="AI13" s="62"/>
+      <c r="AJ13" s="62"/>
+      <c r="AK13" s="62"/>
+      <c r="AL13" s="62"/>
+      <c r="AM13" s="62"/>
+      <c r="AN13" s="63"/>
       <c r="AO13" s="9"/>
       <c r="AP13" s="3"/>
-      <c r="AS13" s="133" t="s">
+      <c r="AS13" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AT13" s="137">
+      <c r="AT13" s="54">
         <v>0</v>
       </c>
-      <c r="AU13" s="137">
+      <c r="AU13" s="54">
         <v>0</v>
       </c>
-      <c r="AV13" s="137">
+      <c r="AV13" s="54">
         <v>2</v>
       </c>
-      <c r="AW13" s="137">
+      <c r="AW13" s="54">
         <v>1</v>
       </c>
-      <c r="AX13" s="137">
+      <c r="AX13" s="54">
         <v>0</v>
       </c>
-      <c r="AY13" s="137">
+      <c r="AY13" s="54">
         <v>0</v>
       </c>
-      <c r="AZ13" s="137">
+      <c r="AZ13" s="54">
         <v>3</v>
       </c>
-      <c r="BA13" s="137">
+      <c r="BA13" s="54">
         <v>0</v>
       </c>
-      <c r="BB13" s="137">
+      <c r="BB13" s="54">
         <v>2</v>
       </c>
-      <c r="BC13" s="137">
+      <c r="BC13" s="54">
         <v>5</v>
       </c>
-      <c r="BD13" s="137">
+      <c r="BD13" s="54">
         <v>0</v>
       </c>
-      <c r="BE13" s="137">
+      <c r="BE13" s="54">
         <v>6</v>
       </c>
-      <c r="BF13" s="137">
+      <c r="BF13" s="54">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="75"/>
-      <c r="M14" s="108"/>
-      <c r="N14" s="74"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="74"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="74"/>
-      <c r="T14" s="75"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="66"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="65"/>
+      <c r="T14" s="66"/>
       <c r="U14" s="8"/>
-      <c r="W14" s="80"/>
-      <c r="X14" s="108"/>
-      <c r="Y14" s="74"/>
-      <c r="Z14" s="74"/>
-      <c r="AA14" s="74"/>
-      <c r="AB14" s="74"/>
-      <c r="AC14" s="74"/>
-      <c r="AD14" s="74"/>
-      <c r="AE14" s="75"/>
-      <c r="AG14" s="108"/>
-      <c r="AH14" s="74"/>
-      <c r="AI14" s="74"/>
-      <c r="AJ14" s="74"/>
-      <c r="AK14" s="74"/>
-      <c r="AL14" s="74"/>
-      <c r="AM14" s="74"/>
-      <c r="AN14" s="75"/>
+      <c r="W14" s="130"/>
+      <c r="X14" s="64"/>
+      <c r="Y14" s="65"/>
+      <c r="Z14" s="65"/>
+      <c r="AA14" s="65"/>
+      <c r="AB14" s="65"/>
+      <c r="AC14" s="65"/>
+      <c r="AD14" s="65"/>
+      <c r="AE14" s="66"/>
+      <c r="AG14" s="64"/>
+      <c r="AH14" s="65"/>
+      <c r="AI14" s="65"/>
+      <c r="AJ14" s="65"/>
+      <c r="AK14" s="65"/>
+      <c r="AL14" s="65"/>
+      <c r="AM14" s="65"/>
+      <c r="AN14" s="66"/>
       <c r="AO14" s="9"/>
       <c r="AP14" s="3"/>
-      <c r="AS14" s="133" t="s">
+      <c r="AS14" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="AT14" s="137">
+      <c r="AT14" s="54">
         <v>0</v>
       </c>
-      <c r="AU14" s="137">
+      <c r="AU14" s="54">
         <v>0</v>
       </c>
-      <c r="AV14" s="137">
+      <c r="AV14" s="54">
         <v>0</v>
       </c>
-      <c r="AW14" s="137">
+      <c r="AW14" s="54">
         <v>1</v>
       </c>
-      <c r="AX14" s="137">
+      <c r="AX14" s="54">
         <v>1</v>
       </c>
-      <c r="AY14" s="137">
+      <c r="AY14" s="54">
         <v>0</v>
       </c>
-      <c r="AZ14" s="137">
+      <c r="AZ14" s="54">
         <v>2</v>
       </c>
-      <c r="BA14" s="137">
+      <c r="BA14" s="54">
         <v>1</v>
       </c>
-      <c r="BB14" s="137">
+      <c r="BB14" s="54">
         <v>1</v>
       </c>
-      <c r="BC14" s="137">
+      <c r="BC14" s="54">
         <v>1</v>
       </c>
-      <c r="BD14" s="137">
+      <c r="BD14" s="54">
         <v>0</v>
       </c>
-      <c r="BE14" s="137">
+      <c r="BE14" s="54">
         <v>2</v>
       </c>
-      <c r="BF14" s="137">
+      <c r="BF14" s="54">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
-      <c r="C15" s="77"/>
+      <c r="C15" s="127"/>
       <c r="U15" s="8"/>
-      <c r="W15" s="80"/>
+      <c r="W15" s="130"/>
       <c r="AO15" s="9"/>
       <c r="AP15" s="3"/>
-      <c r="AT15" s="138">
+      <c r="AT15" s="93">
         <v>43646</v>
       </c>
-      <c r="AU15" s="138">
+      <c r="AU15" s="93">
         <v>43677</v>
       </c>
-      <c r="AV15" s="138">
+      <c r="AV15" s="93">
         <v>43708</v>
       </c>
-      <c r="AW15" s="138">
+      <c r="AW15" s="93">
         <v>43738</v>
       </c>
-      <c r="AX15" s="138">
+      <c r="AX15" s="93">
         <v>43769</v>
       </c>
-      <c r="AY15" s="138">
+      <c r="AY15" s="93">
         <v>43799</v>
       </c>
-      <c r="AZ15" s="138">
+      <c r="AZ15" s="93">
         <v>43830</v>
       </c>
-      <c r="BA15" s="138">
+      <c r="BA15" s="93">
         <v>43861</v>
       </c>
-      <c r="BB15" s="138">
+      <c r="BB15" s="93">
         <v>43890</v>
       </c>
-      <c r="BC15" s="138">
+      <c r="BC15" s="93">
         <v>43921</v>
       </c>
-      <c r="BD15" s="138">
+      <c r="BD15" s="93">
         <v>43951</v>
       </c>
-      <c r="BE15" s="138">
+      <c r="BE15" s="93">
         <v>43982</v>
       </c>
-      <c r="BF15" s="134" t="s">
+      <c r="BF15" s="92" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="82" t="s">
+      <c r="C16" s="127"/>
+      <c r="D16" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="91">
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="117">
         <v>0.60897012673056483</v>
       </c>
-      <c r="K16" s="92"/>
-      <c r="M16" s="89" t="s">
+      <c r="K16" s="118"/>
+      <c r="M16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="83"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="52"/>
-      <c r="S16" s="91">
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="117">
         <v>0.51899473632415571</v>
       </c>
-      <c r="T16" s="92"/>
+      <c r="T16" s="118"/>
       <c r="U16" s="8"/>
-      <c r="W16" s="80"/>
-      <c r="X16" s="102" t="s">
+      <c r="W16" s="130"/>
+      <c r="X16" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="Y16" s="83"/>
-      <c r="Z16" s="83"/>
-      <c r="AA16" s="83"/>
-      <c r="AB16" s="51"/>
-      <c r="AC16" s="52"/>
-      <c r="AD16" s="103">
+      <c r="Y16" s="68"/>
+      <c r="Z16" s="68"/>
+      <c r="AA16" s="68"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="72"/>
+      <c r="AD16" s="82">
         <v>73</v>
       </c>
-      <c r="AE16" s="104"/>
-      <c r="AG16" s="102" t="s">
+      <c r="AE16" s="83"/>
+      <c r="AG16" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="AH16" s="83"/>
-      <c r="AI16" s="83"/>
-      <c r="AJ16" s="83"/>
-      <c r="AK16" s="51"/>
-      <c r="AL16" s="52"/>
-      <c r="AM16" s="63">
+      <c r="AH16" s="68"/>
+      <c r="AI16" s="68"/>
+      <c r="AJ16" s="68"/>
+      <c r="AK16" s="71"/>
+      <c r="AL16" s="72"/>
+      <c r="AM16" s="112">
         <f>BB33</f>
         <v>7</v>
       </c>
-      <c r="AN16" s="64"/>
+      <c r="AN16" s="113"/>
       <c r="AO16" s="9"/>
       <c r="AP16" s="3"/>
-      <c r="AS16" s="139"/>
-      <c r="AT16" s="138"/>
-      <c r="AU16" s="138"/>
-      <c r="AV16" s="138"/>
-      <c r="AW16" s="138"/>
-      <c r="AX16" s="138"/>
-      <c r="AY16" s="138"/>
-      <c r="AZ16" s="138"/>
-      <c r="BA16" s="138"/>
-      <c r="BB16" s="138"/>
-      <c r="BC16" s="138"/>
-      <c r="BD16" s="138"/>
-      <c r="BE16" s="138"/>
-      <c r="BF16" s="134"/>
+      <c r="AS16" s="55"/>
+      <c r="AT16" s="93"/>
+      <c r="AU16" s="93"/>
+      <c r="AV16" s="93"/>
+      <c r="AW16" s="93"/>
+      <c r="AX16" s="93"/>
+      <c r="AY16" s="93"/>
+      <c r="AZ16" s="93"/>
+      <c r="BA16" s="93"/>
+      <c r="BB16" s="93"/>
+      <c r="BC16" s="93"/>
+      <c r="BD16" s="93"/>
+      <c r="BE16" s="93"/>
+      <c r="BF16" s="92"/>
     </row>
     <row r="17" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="94"/>
-      <c r="M17" s="90"/>
-      <c r="N17" s="84"/>
-      <c r="O17" s="84"/>
-      <c r="P17" s="84"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="93"/>
-      <c r="T17" s="94"/>
+      <c r="C17" s="127"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="120"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
+      <c r="Q17" s="73"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="120"/>
       <c r="U17" s="8"/>
-      <c r="W17" s="80"/>
-      <c r="X17" s="90"/>
-      <c r="Y17" s="84"/>
-      <c r="Z17" s="84"/>
-      <c r="AA17" s="84"/>
-      <c r="AB17" s="53"/>
-      <c r="AC17" s="54"/>
-      <c r="AD17" s="105"/>
-      <c r="AE17" s="106"/>
-      <c r="AG17" s="90"/>
-      <c r="AH17" s="84"/>
-      <c r="AI17" s="84"/>
-      <c r="AJ17" s="84"/>
-      <c r="AK17" s="53"/>
-      <c r="AL17" s="54"/>
-      <c r="AM17" s="65"/>
-      <c r="AN17" s="66"/>
+      <c r="W17" s="130"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="70"/>
+      <c r="Z17" s="70"/>
+      <c r="AA17" s="70"/>
+      <c r="AB17" s="73"/>
+      <c r="AC17" s="74"/>
+      <c r="AD17" s="84"/>
+      <c r="AE17" s="85"/>
+      <c r="AG17" s="69"/>
+      <c r="AH17" s="70"/>
+      <c r="AI17" s="70"/>
+      <c r="AJ17" s="70"/>
+      <c r="AK17" s="73"/>
+      <c r="AL17" s="74"/>
+      <c r="AM17" s="114"/>
+      <c r="AN17" s="115"/>
       <c r="AO17" s="9"/>
       <c r="AP17" s="3"/>
-      <c r="AS17" s="139"/>
-      <c r="AT17" s="138"/>
-      <c r="AU17" s="138"/>
-      <c r="AV17" s="138"/>
-      <c r="AW17" s="138"/>
-      <c r="AX17" s="138"/>
-      <c r="AY17" s="138"/>
-      <c r="AZ17" s="138"/>
-      <c r="BA17" s="138"/>
-      <c r="BB17" s="138"/>
-      <c r="BC17" s="138"/>
-      <c r="BD17" s="138"/>
-      <c r="BE17" s="138"/>
-      <c r="BF17" s="134"/>
+      <c r="AS17" s="55"/>
+      <c r="AT17" s="93"/>
+      <c r="AU17" s="93"/>
+      <c r="AV17" s="93"/>
+      <c r="AW17" s="93"/>
+      <c r="AX17" s="93"/>
+      <c r="AY17" s="93"/>
+      <c r="AZ17" s="93"/>
+      <c r="BA17" s="93"/>
+      <c r="BB17" s="93"/>
+      <c r="BC17" s="93"/>
+      <c r="BD17" s="93"/>
+      <c r="BE17" s="93"/>
+      <c r="BF17" s="92"/>
     </row>
     <row r="18" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="94"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="84"/>
-      <c r="O18" s="84"/>
-      <c r="P18" s="84"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="56"/>
-      <c r="S18" s="93"/>
-      <c r="T18" s="94"/>
+      <c r="C18" s="127"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="120"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="70"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="76"/>
+      <c r="S18" s="119"/>
+      <c r="T18" s="120"/>
       <c r="U18" s="8"/>
-      <c r="W18" s="80"/>
-      <c r="X18" s="90"/>
-      <c r="Y18" s="84"/>
-      <c r="Z18" s="84"/>
-      <c r="AA18" s="84"/>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="56"/>
-      <c r="AD18" s="105"/>
-      <c r="AE18" s="106"/>
-      <c r="AG18" s="90"/>
-      <c r="AH18" s="84"/>
-      <c r="AI18" s="84"/>
-      <c r="AJ18" s="84"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="56"/>
-      <c r="AM18" s="65"/>
-      <c r="AN18" s="66"/>
+      <c r="W18" s="130"/>
+      <c r="X18" s="69"/>
+      <c r="Y18" s="70"/>
+      <c r="Z18" s="70"/>
+      <c r="AA18" s="70"/>
+      <c r="AB18" s="75"/>
+      <c r="AC18" s="76"/>
+      <c r="AD18" s="84"/>
+      <c r="AE18" s="85"/>
+      <c r="AG18" s="69"/>
+      <c r="AH18" s="70"/>
+      <c r="AI18" s="70"/>
+      <c r="AJ18" s="70"/>
+      <c r="AK18" s="75"/>
+      <c r="AL18" s="76"/>
+      <c r="AM18" s="114"/>
+      <c r="AN18" s="115"/>
       <c r="AO18" s="9"/>
       <c r="AP18" s="3"/>
-      <c r="AS18" s="139"/>
-      <c r="AT18" s="140"/>
-      <c r="AU18" s="140"/>
-      <c r="AV18" s="140"/>
-      <c r="AW18" s="140"/>
-      <c r="AX18" s="140"/>
-      <c r="AY18" s="140"/>
-      <c r="AZ18" s="140"/>
-      <c r="BA18" s="140"/>
-      <c r="BB18" s="140"/>
-      <c r="BC18" s="140"/>
-      <c r="BD18" s="140"/>
-      <c r="BE18" s="140"/>
-      <c r="BF18" s="141"/>
+      <c r="AS18" s="55"/>
+      <c r="AT18" s="56"/>
+      <c r="AU18" s="56"/>
+      <c r="AV18" s="56"/>
+      <c r="AW18" s="56"/>
+      <c r="AX18" s="56"/>
+      <c r="AY18" s="56"/>
+      <c r="AZ18" s="56"/>
+      <c r="BA18" s="56"/>
+      <c r="BB18" s="56"/>
+      <c r="BC18" s="56"/>
+      <c r="BD18" s="56"/>
+      <c r="BE18" s="56"/>
+      <c r="BF18" s="57"/>
     </row>
     <row r="19" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="72" t="s">
+      <c r="C19" s="127"/>
+      <c r="D19" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="73"/>
-      <c r="M19" s="107" t="s">
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="63"/>
+      <c r="M19" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="72"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="72"/>
-      <c r="R19" s="72"/>
-      <c r="S19" s="72"/>
-      <c r="T19" s="73"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="63"/>
       <c r="U19" s="8"/>
-      <c r="W19" s="80"/>
-      <c r="X19" s="107" t="s">
+      <c r="W19" s="130"/>
+      <c r="X19" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="Y19" s="72"/>
-      <c r="Z19" s="72"/>
-      <c r="AA19" s="72"/>
-      <c r="AB19" s="72"/>
-      <c r="AC19" s="72"/>
-      <c r="AD19" s="72"/>
-      <c r="AE19" s="73"/>
-      <c r="AG19" s="107" t="s">
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="62"/>
+      <c r="AA19" s="62"/>
+      <c r="AB19" s="62"/>
+      <c r="AC19" s="62"/>
+      <c r="AD19" s="62"/>
+      <c r="AE19" s="63"/>
+      <c r="AG19" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="AH19" s="72"/>
-      <c r="AI19" s="72"/>
-      <c r="AJ19" s="72"/>
-      <c r="AK19" s="72"/>
-      <c r="AL19" s="72"/>
-      <c r="AM19" s="72"/>
-      <c r="AN19" s="73"/>
+      <c r="AH19" s="62"/>
+      <c r="AI19" s="62"/>
+      <c r="AJ19" s="62"/>
+      <c r="AK19" s="62"/>
+      <c r="AL19" s="62"/>
+      <c r="AM19" s="62"/>
+      <c r="AN19" s="63"/>
       <c r="AO19" s="9"/>
       <c r="AP19" s="3"/>
     </row>
     <row r="20" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="75"/>
-      <c r="M20" s="108"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74"/>
-      <c r="S20" s="74"/>
-      <c r="T20" s="75"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="66"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="65"/>
+      <c r="T20" s="66"/>
       <c r="U20" s="8"/>
-      <c r="W20" s="80"/>
-      <c r="X20" s="108"/>
-      <c r="Y20" s="74"/>
-      <c r="Z20" s="74"/>
-      <c r="AA20" s="74"/>
-      <c r="AB20" s="74"/>
-      <c r="AC20" s="74"/>
-      <c r="AD20" s="74"/>
-      <c r="AE20" s="75"/>
-      <c r="AG20" s="108"/>
-      <c r="AH20" s="74"/>
-      <c r="AI20" s="74"/>
-      <c r="AJ20" s="74"/>
-      <c r="AK20" s="74"/>
-      <c r="AL20" s="74"/>
-      <c r="AM20" s="74"/>
-      <c r="AN20" s="75"/>
+      <c r="W20" s="130"/>
+      <c r="X20" s="64"/>
+      <c r="Y20" s="65"/>
+      <c r="Z20" s="65"/>
+      <c r="AA20" s="65"/>
+      <c r="AB20" s="65"/>
+      <c r="AC20" s="65"/>
+      <c r="AD20" s="65"/>
+      <c r="AE20" s="66"/>
+      <c r="AG20" s="64"/>
+      <c r="AH20" s="65"/>
+      <c r="AI20" s="65"/>
+      <c r="AJ20" s="65"/>
+      <c r="AK20" s="65"/>
+      <c r="AL20" s="65"/>
+      <c r="AM20" s="65"/>
+      <c r="AN20" s="66"/>
       <c r="AO20" s="9"/>
       <c r="AP20" s="3"/>
     </row>
     <row r="21" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
-      <c r="C21" s="78"/>
+      <c r="C21" s="128"/>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -8501,7 +8459,7 @@
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
       <c r="U21" s="13"/>
-      <c r="W21" s="81"/>
+      <c r="W21" s="131"/>
       <c r="X21" s="14"/>
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
@@ -8521,37 +8479,37 @@
       <c r="AN21" s="14"/>
       <c r="AO21" s="15"/>
       <c r="AP21" s="3"/>
-      <c r="AW21" s="142" t="s">
+      <c r="AW21" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="AX21" s="142" t="s">
+      <c r="AX21" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="AY21" s="142" t="s">
+      <c r="AY21" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="AZ21" s="142" t="s">
+      <c r="AZ21" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BA21" s="142" t="s">
+      <c r="BA21" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="BB21" s="142" t="s">
+      <c r="BB21" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="BD21" s="133" t="s">
+      <c r="BD21" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="BE21" s="133" t="s">
+      <c r="BE21" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="BF21" s="133" t="s">
+      <c r="BF21" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="BG21" s="133" t="s">
+      <c r="BG21" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="BH21" s="133" t="s">
+      <c r="BH21" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -8569,46 +8527,46 @@
       <c r="AN22" s="16"/>
       <c r="AO22" s="16"/>
       <c r="AP22" s="3"/>
-      <c r="AS22" s="133" t="s">
+      <c r="AS22" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="AW22" s="143">
+      <c r="AW22" s="59">
         <v>0.2</v>
       </c>
-      <c r="AX22" s="143">
+      <c r="AX22" s="59">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AY22" s="143">
+      <c r="AY22" s="59">
         <v>0.75</v>
       </c>
-      <c r="AZ22" s="143">
+      <c r="AZ22" s="59">
         <v>1</v>
       </c>
-      <c r="BA22" s="143">
+      <c r="BA22" s="59">
         <v>0.88</v>
       </c>
-      <c r="BB22" s="143">
+      <c r="BB22" s="59">
         <v>0.88</v>
       </c>
-      <c r="BD22" s="133" t="s">
+      <c r="BD22" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="BE22" s="133" t="s">
+      <c r="BE22" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="BF22" s="133" t="s">
+      <c r="BF22" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="BG22" s="133" t="s">
+      <c r="BG22" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="BH22" s="133" t="s">
+      <c r="BH22" s="51" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="94" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="17"/>
@@ -8639,446 +8597,446 @@
       <c r="AC23" s="17"/>
       <c r="AD23" s="18"/>
       <c r="AE23" s="19"/>
-      <c r="AF23" s="112" t="s">
+      <c r="AF23" s="97" t="s">
         <v>42</v>
       </c>
       <c r="AO23" s="20"/>
       <c r="AP23" s="3"/>
-      <c r="AS23" s="133" t="s">
+      <c r="AS23" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AW23" s="133">
+      <c r="AW23" s="51">
         <v>302400</v>
       </c>
-      <c r="AX23" s="133">
+      <c r="AX23" s="51">
         <v>504000</v>
       </c>
-      <c r="AY23" s="133">
+      <c r="AY23" s="51">
         <v>376200</v>
       </c>
-      <c r="AZ23" s="133">
+      <c r="AZ23" s="51">
         <v>347400</v>
       </c>
-      <c r="BA23" s="133">
+      <c r="BA23" s="51">
         <v>601200</v>
       </c>
-      <c r="BB23" s="133">
+      <c r="BB23" s="51">
         <v>601200</v>
       </c>
-      <c r="BD23" s="133" t="s">
+      <c r="BD23" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="BE23" s="133" t="s">
+      <c r="BE23" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="BF23" s="133" t="s">
+      <c r="BF23" s="51" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
-      <c r="C24" s="110"/>
-      <c r="D24" s="132">
+      <c r="C24" s="95"/>
+      <c r="D24" s="111">
         <f>SUM(AT5:AW5)</f>
         <v>16</v>
       </c>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="132"/>
-      <c r="H24" s="132"/>
-      <c r="I24" s="132"/>
-      <c r="J24" s="132"/>
-      <c r="K24" s="132"/>
-      <c r="L24" s="132"/>
-      <c r="M24" s="132"/>
-      <c r="N24" s="132"/>
-      <c r="O24" s="114" t="str">
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="111"/>
+      <c r="M24" s="111"/>
+      <c r="N24" s="111"/>
+      <c r="O24" s="99" t="str">
         <f>"Release Velocity "&amp;CHAR(10)&amp;TEXT(AS4,"dd-mmm")</f>
         <v>Release Velocity 
 10-Jun</v>
       </c>
-      <c r="P24" s="115"/>
-      <c r="Q24" s="115"/>
-      <c r="R24" s="115"/>
-      <c r="S24" s="130" t="s">
+      <c r="P24" s="100"/>
+      <c r="Q24" s="100"/>
+      <c r="R24" s="100"/>
+      <c r="S24" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="T24" s="131"/>
-      <c r="V24" s="102" t="s">
+      <c r="T24" s="91"/>
+      <c r="V24" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="W24" s="83"/>
-      <c r="X24" s="83"/>
-      <c r="Y24" s="83"/>
-      <c r="Z24" s="118"/>
-      <c r="AA24" s="119"/>
-      <c r="AB24" s="122">
+      <c r="W24" s="68"/>
+      <c r="X24" s="68"/>
+      <c r="Y24" s="68"/>
+      <c r="Z24" s="103"/>
+      <c r="AA24" s="104"/>
+      <c r="AB24" s="107">
         <f>BB35</f>
         <v>1.3620751316435028E-2</v>
       </c>
-      <c r="AC24" s="123"/>
+      <c r="AC24" s="108"/>
       <c r="AD24" s="21"/>
       <c r="AE24" s="19"/>
-      <c r="AF24" s="112"/>
-      <c r="AG24" s="89" t="s">
+      <c r="AF24" s="97"/>
+      <c r="AG24" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="AH24" s="83"/>
-      <c r="AI24" s="83"/>
-      <c r="AJ24" s="83"/>
-      <c r="AK24" s="51"/>
-      <c r="AL24" s="52"/>
-      <c r="AM24" s="103">
+      <c r="AH24" s="68"/>
+      <c r="AI24" s="68"/>
+      <c r="AJ24" s="68"/>
+      <c r="AK24" s="71"/>
+      <c r="AL24" s="72"/>
+      <c r="AM24" s="82">
         <f>BB37</f>
         <v>137.6</v>
       </c>
-      <c r="AN24" s="104"/>
+      <c r="AN24" s="83"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="3"/>
     </row>
     <row r="25" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="132"/>
-      <c r="H25" s="132"/>
-      <c r="I25" s="132"/>
-      <c r="J25" s="132"/>
-      <c r="K25" s="132"/>
-      <c r="L25" s="132"/>
-      <c r="M25" s="132"/>
-      <c r="N25" s="132"/>
-      <c r="O25" s="116"/>
-      <c r="P25" s="117"/>
-      <c r="Q25" s="117"/>
-      <c r="R25" s="117"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="111"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="111"/>
+      <c r="J25" s="111"/>
+      <c r="K25" s="111"/>
+      <c r="L25" s="111"/>
+      <c r="M25" s="111"/>
+      <c r="N25" s="111"/>
+      <c r="O25" s="101"/>
+      <c r="P25" s="102"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="102"/>
       <c r="S25" s="22" t="s">
         <v>17</v>
       </c>
       <c r="T25" s="23"/>
-      <c r="V25" s="90"/>
-      <c r="W25" s="84"/>
-      <c r="X25" s="84"/>
-      <c r="Y25" s="84"/>
-      <c r="Z25" s="120"/>
-      <c r="AA25" s="121"/>
-      <c r="AB25" s="124"/>
-      <c r="AC25" s="125"/>
+      <c r="V25" s="69"/>
+      <c r="W25" s="70"/>
+      <c r="X25" s="70"/>
+      <c r="Y25" s="70"/>
+      <c r="Z25" s="105"/>
+      <c r="AA25" s="106"/>
+      <c r="AB25" s="109"/>
+      <c r="AC25" s="110"/>
       <c r="AD25" s="21"/>
       <c r="AE25" s="19"/>
-      <c r="AF25" s="112"/>
-      <c r="AG25" s="90"/>
-      <c r="AH25" s="84"/>
-      <c r="AI25" s="84"/>
-      <c r="AJ25" s="84"/>
-      <c r="AK25" s="53"/>
-      <c r="AL25" s="54"/>
-      <c r="AM25" s="105"/>
-      <c r="AN25" s="106"/>
+      <c r="AF25" s="97"/>
+      <c r="AG25" s="69"/>
+      <c r="AH25" s="70"/>
+      <c r="AI25" s="70"/>
+      <c r="AJ25" s="70"/>
+      <c r="AK25" s="73"/>
+      <c r="AL25" s="74"/>
+      <c r="AM25" s="84"/>
+      <c r="AN25" s="85"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="3"/>
-      <c r="AS25" s="133" t="s">
+      <c r="AS25" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="AW25" s="137">
+      <c r="AW25" s="54">
         <v>32.46987951807229</v>
       </c>
-      <c r="AX25" s="137">
+      <c r="AX25" s="54">
         <v>39.769230769230766</v>
       </c>
-      <c r="AY25" s="137">
+      <c r="AY25" s="54">
         <v>27.166666666666668</v>
       </c>
-      <c r="AZ25" s="137">
+      <c r="AZ25" s="54">
         <v>14</v>
       </c>
-      <c r="BA25" s="137">
+      <c r="BA25" s="54">
         <v>17</v>
       </c>
-      <c r="BB25" s="137">
+      <c r="BB25" s="54">
         <v>20</v>
       </c>
-      <c r="BD25" s="133" t="s">
+      <c r="BD25" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="BE25" s="133" t="s">
+      <c r="BE25" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="BF25" s="133" t="s">
+      <c r="BF25" s="51" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
-      <c r="C26" s="110"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="132"/>
-      <c r="H26" s="132"/>
-      <c r="I26" s="132"/>
-      <c r="J26" s="132"/>
-      <c r="K26" s="132"/>
-      <c r="L26" s="132"/>
-      <c r="M26" s="132"/>
-      <c r="N26" s="132"/>
-      <c r="O26" s="116"/>
-      <c r="P26" s="117"/>
-      <c r="Q26" s="117"/>
-      <c r="R26" s="117"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="111"/>
+      <c r="H26" s="111"/>
+      <c r="I26" s="111"/>
+      <c r="J26" s="111"/>
+      <c r="K26" s="111"/>
+      <c r="L26" s="111"/>
+      <c r="M26" s="111"/>
+      <c r="N26" s="111"/>
+      <c r="O26" s="101"/>
+      <c r="P26" s="102"/>
+      <c r="Q26" s="102"/>
+      <c r="R26" s="102"/>
       <c r="S26" s="22" t="s">
         <v>1</v>
       </c>
       <c r="T26" s="23"/>
-      <c r="V26" s="90"/>
-      <c r="W26" s="84"/>
-      <c r="X26" s="84"/>
-      <c r="Y26" s="84"/>
-      <c r="Z26" s="120"/>
-      <c r="AA26" s="121"/>
-      <c r="AB26" s="124"/>
-      <c r="AC26" s="125"/>
+      <c r="V26" s="69"/>
+      <c r="W26" s="70"/>
+      <c r="X26" s="70"/>
+      <c r="Y26" s="70"/>
+      <c r="Z26" s="105"/>
+      <c r="AA26" s="106"/>
+      <c r="AB26" s="109"/>
+      <c r="AC26" s="110"/>
       <c r="AD26" s="21"/>
       <c r="AE26" s="19"/>
-      <c r="AF26" s="112"/>
-      <c r="AG26" s="90"/>
-      <c r="AH26" s="84"/>
-      <c r="AI26" s="84"/>
-      <c r="AJ26" s="84"/>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="56"/>
-      <c r="AM26" s="105"/>
-      <c r="AN26" s="106"/>
+      <c r="AF26" s="97"/>
+      <c r="AG26" s="69"/>
+      <c r="AH26" s="70"/>
+      <c r="AI26" s="70"/>
+      <c r="AJ26" s="70"/>
+      <c r="AK26" s="75"/>
+      <c r="AL26" s="76"/>
+      <c r="AM26" s="84"/>
+      <c r="AN26" s="85"/>
       <c r="AO26" s="19"/>
       <c r="AP26" s="3"/>
-      <c r="AS26" s="133" t="s">
+      <c r="AS26" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="AW26" s="143">
+      <c r="AW26" s="59">
         <v>5.1724137931034482E-2</v>
       </c>
-      <c r="AX26" s="143">
+      <c r="AX26" s="59">
         <v>0.26315789473684209</v>
       </c>
-      <c r="AY26" s="143">
+      <c r="AY26" s="59">
         <v>0.64150943396226412</v>
       </c>
-      <c r="AZ26" s="143">
+      <c r="AZ26" s="59">
         <v>1</v>
       </c>
-      <c r="BA26" s="143">
+      <c r="BA26" s="59">
         <v>0.83783783783783783</v>
       </c>
-      <c r="BB26" s="143">
+      <c r="BB26" s="59">
         <v>0.46666666666666667</v>
       </c>
-      <c r="BD26" s="133" t="s">
+      <c r="BD26" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="BE26" s="133" t="s">
+      <c r="BE26" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="BF26" s="133" t="s">
+      <c r="BF26" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="BG26" s="133" t="s">
+      <c r="BG26" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="BH26" s="133" t="s">
+      <c r="BH26" s="51" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132"/>
-      <c r="G27" s="132"/>
-      <c r="H27" s="132"/>
-      <c r="I27" s="132"/>
-      <c r="J27" s="132"/>
-      <c r="K27" s="132"/>
-      <c r="L27" s="132"/>
-      <c r="M27" s="132"/>
-      <c r="N27" s="132"/>
-      <c r="O27" s="126" t="s">
+      <c r="C27" s="95"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="111"/>
+      <c r="H27" s="111"/>
+      <c r="I27" s="111"/>
+      <c r="J27" s="111"/>
+      <c r="K27" s="111"/>
+      <c r="L27" s="111"/>
+      <c r="M27" s="111"/>
+      <c r="N27" s="111"/>
+      <c r="O27" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="P27" s="127"/>
-      <c r="Q27" s="127"/>
-      <c r="R27" s="127"/>
+      <c r="P27" s="87"/>
+      <c r="Q27" s="87"/>
+      <c r="R27" s="87"/>
       <c r="S27" s="22" t="s">
         <v>2</v>
       </c>
       <c r="T27" s="23"/>
-      <c r="V27" s="126" t="str">
+      <c r="V27" s="86" t="str">
         <f xml:space="preserve"> "Average of Active Time ("&amp;BB43&amp;" days) / Lead Team for the issues released in the last 3 months"</f>
         <v>Average of Active Time (2.1 days) / Lead Team for the issues released in the last 3 months</v>
       </c>
-      <c r="W27" s="127"/>
-      <c r="X27" s="127"/>
-      <c r="Y27" s="127"/>
-      <c r="Z27" s="127"/>
-      <c r="AA27" s="127"/>
-      <c r="AB27" s="127"/>
-      <c r="AC27" s="127"/>
+      <c r="W27" s="87"/>
+      <c r="X27" s="87"/>
+      <c r="Y27" s="87"/>
+      <c r="Z27" s="87"/>
+      <c r="AA27" s="87"/>
+      <c r="AB27" s="87"/>
+      <c r="AC27" s="87"/>
       <c r="AD27" s="21"/>
       <c r="AE27" s="19"/>
-      <c r="AF27" s="112"/>
-      <c r="AG27" s="107" t="s">
+      <c r="AF27" s="97"/>
+      <c r="AG27" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="AH27" s="72"/>
-      <c r="AI27" s="72"/>
-      <c r="AJ27" s="72"/>
-      <c r="AK27" s="72"/>
-      <c r="AL27" s="72"/>
-      <c r="AM27" s="72"/>
-      <c r="AN27" s="73"/>
+      <c r="AH27" s="62"/>
+      <c r="AI27" s="62"/>
+      <c r="AJ27" s="62"/>
+      <c r="AK27" s="62"/>
+      <c r="AL27" s="62"/>
+      <c r="AM27" s="62"/>
+      <c r="AN27" s="63"/>
       <c r="AO27" s="19"/>
       <c r="AP27" s="3"/>
-      <c r="AS27" s="133" t="s">
+      <c r="AS27" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="AW27" s="144">
+      <c r="AW27" s="60">
         <v>0.76029542340884804</v>
       </c>
-      <c r="AX27" s="144">
+      <c r="AX27" s="60">
         <v>0.76029542340884804</v>
       </c>
-      <c r="AY27" s="144">
+      <c r="AY27" s="60">
         <v>0.79120337968461985</v>
       </c>
-      <c r="AZ27" s="144">
+      <c r="AZ27" s="60">
         <v>0.84008886045782594</v>
       </c>
-      <c r="BA27" s="144">
+      <c r="BA27" s="60">
         <v>1.3221664701611811</v>
       </c>
-      <c r="BB27" s="144">
+      <c r="BB27" s="60">
         <v>0.60897012673056483</v>
       </c>
-      <c r="BD27" s="133" t="s">
+      <c r="BD27" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="BE27" s="133" t="s">
+      <c r="BE27" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="BF27" s="133" t="s">
+      <c r="BF27" s="51" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
-      <c r="C28" s="110"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="132"/>
-      <c r="F28" s="132"/>
-      <c r="G28" s="132"/>
-      <c r="H28" s="132"/>
-      <c r="I28" s="132"/>
-      <c r="J28" s="132"/>
-      <c r="K28" s="132"/>
-      <c r="L28" s="132"/>
-      <c r="M28" s="132"/>
-      <c r="N28" s="132"/>
-      <c r="O28" s="128"/>
-      <c r="P28" s="129"/>
-      <c r="Q28" s="129"/>
-      <c r="R28" s="129"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="111"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="111"/>
+      <c r="M28" s="111"/>
+      <c r="N28" s="111"/>
+      <c r="O28" s="88"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="89"/>
+      <c r="R28" s="89"/>
       <c r="S28" s="25" t="s">
         <v>3</v>
       </c>
       <c r="T28" s="26"/>
-      <c r="V28" s="126"/>
-      <c r="W28" s="127"/>
-      <c r="X28" s="127"/>
-      <c r="Y28" s="127"/>
-      <c r="Z28" s="127"/>
-      <c r="AA28" s="127"/>
-      <c r="AB28" s="127"/>
-      <c r="AC28" s="127"/>
+      <c r="V28" s="86"/>
+      <c r="W28" s="87"/>
+      <c r="X28" s="87"/>
+      <c r="Y28" s="87"/>
+      <c r="Z28" s="87"/>
+      <c r="AA28" s="87"/>
+      <c r="AB28" s="87"/>
+      <c r="AC28" s="87"/>
       <c r="AD28" s="21"/>
       <c r="AE28" s="19"/>
-      <c r="AF28" s="112"/>
-      <c r="AG28" s="108"/>
-      <c r="AH28" s="74"/>
-      <c r="AI28" s="74"/>
-      <c r="AJ28" s="74"/>
-      <c r="AK28" s="74"/>
-      <c r="AL28" s="74"/>
-      <c r="AM28" s="74"/>
-      <c r="AN28" s="75"/>
+      <c r="AF28" s="97"/>
+      <c r="AG28" s="64"/>
+      <c r="AH28" s="65"/>
+      <c r="AI28" s="65"/>
+      <c r="AJ28" s="65"/>
+      <c r="AK28" s="65"/>
+      <c r="AL28" s="65"/>
+      <c r="AM28" s="65"/>
+      <c r="AN28" s="66"/>
       <c r="AO28" s="19"/>
       <c r="AP28" s="3"/>
-      <c r="AS28" s="133" t="s">
+      <c r="AS28" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="AW28" s="143">
+      <c r="AW28" s="59">
         <v>1.1791440964995212</v>
       </c>
-      <c r="AX28" s="143">
+      <c r="AX28" s="59">
         <v>1.0117651106127619</v>
       </c>
-      <c r="AY28" s="143">
+      <c r="AY28" s="59">
         <v>0.98287811183078511</v>
       </c>
-      <c r="AZ28" s="143">
+      <c r="AZ28" s="59">
         <v>0.72482845074783719</v>
       </c>
-      <c r="BA28" s="143">
+      <c r="BA28" s="59">
         <v>0.76394336665463713</v>
       </c>
-      <c r="BB28" s="143">
+      <c r="BB28" s="59">
         <v>0.51899473632415571</v>
       </c>
-      <c r="BD28" s="133" t="s">
+      <c r="BD28" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="BE28" s="133" t="s">
+      <c r="BE28" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="BF28" s="133" t="s">
+      <c r="BF28" s="51" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="29" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
-      <c r="G29" s="132"/>
-      <c r="H29" s="132"/>
-      <c r="I29" s="132"/>
-      <c r="J29" s="132"/>
-      <c r="K29" s="132"/>
-      <c r="L29" s="132"/>
-      <c r="M29" s="132"/>
-      <c r="N29" s="132"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="111"/>
+      <c r="H29" s="111"/>
+      <c r="I29" s="111"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="111"/>
+      <c r="L29" s="111"/>
+      <c r="M29" s="111"/>
+      <c r="N29" s="111"/>
       <c r="AD29" s="21"/>
       <c r="AE29" s="19"/>
-      <c r="AF29" s="112"/>
+      <c r="AF29" s="97"/>
       <c r="AO29" s="19"/>
       <c r="AP29" s="3"/>
     </row>
     <row r="30" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="132"/>
-      <c r="F30" s="132"/>
-      <c r="G30" s="132"/>
-      <c r="H30" s="132"/>
-      <c r="I30" s="132"/>
-      <c r="J30" s="132"/>
-      <c r="K30" s="132"/>
-      <c r="L30" s="132"/>
-      <c r="M30" s="132"/>
-      <c r="N30" s="132"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="111"/>
+      <c r="F30" s="111"/>
+      <c r="G30" s="111"/>
+      <c r="H30" s="111"/>
+      <c r="I30" s="111"/>
+      <c r="J30" s="111"/>
+      <c r="K30" s="111"/>
+      <c r="L30" s="111"/>
+      <c r="M30" s="111"/>
+      <c r="N30" s="111"/>
       <c r="P30" s="27"/>
       <c r="Q30" s="28"/>
       <c r="R30" s="28"/>
@@ -9097,57 +9055,57 @@
       </c>
       <c r="AD30" s="21"/>
       <c r="AE30" s="19"/>
-      <c r="AF30" s="112"/>
-      <c r="AG30" s="102" t="s">
+      <c r="AF30" s="97"/>
+      <c r="AG30" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="AH30" s="83"/>
-      <c r="AI30" s="83"/>
-      <c r="AJ30" s="83"/>
-      <c r="AK30" s="51"/>
-      <c r="AL30" s="52"/>
-      <c r="AM30" s="145">
+      <c r="AH30" s="68"/>
+      <c r="AI30" s="68"/>
+      <c r="AJ30" s="68"/>
+      <c r="AK30" s="71"/>
+      <c r="AL30" s="72"/>
+      <c r="AM30" s="77">
         <v>0.01</v>
       </c>
-      <c r="AN30" s="146"/>
+      <c r="AN30" s="78"/>
       <c r="AO30" s="19"/>
       <c r="AP30" s="3"/>
-      <c r="AS30" s="133" t="s">
+      <c r="AS30" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AW30" s="133">
+      <c r="AW30" s="51">
         <v>108.76923076923077</v>
       </c>
-      <c r="AX30" s="133">
+      <c r="AX30" s="51">
         <v>108.76923076923077</v>
       </c>
-      <c r="AY30" s="133">
+      <c r="AY30" s="51">
         <v>131.11111111111111</v>
       </c>
-      <c r="AZ30" s="133">
+      <c r="AZ30" s="51">
         <v>133.5</v>
       </c>
-      <c r="BA30" s="133">
+      <c r="BA30" s="51">
         <v>110.45454545454545</v>
       </c>
-      <c r="BB30" s="133">
+      <c r="BB30" s="51">
         <v>155.77272727272728</v>
       </c>
     </row>
     <row r="31" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
-      <c r="C31" s="110"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="132"/>
-      <c r="G31" s="132"/>
-      <c r="H31" s="132"/>
-      <c r="I31" s="132"/>
-      <c r="J31" s="132"/>
-      <c r="K31" s="132"/>
-      <c r="L31" s="132"/>
-      <c r="M31" s="132"/>
-      <c r="N31" s="132"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="111"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="111"/>
+      <c r="G31" s="111"/>
+      <c r="H31" s="111"/>
+      <c r="I31" s="111"/>
+      <c r="J31" s="111"/>
+      <c r="K31" s="111"/>
+      <c r="L31" s="111"/>
+      <c r="M31" s="111"/>
+      <c r="N31" s="111"/>
       <c r="P31" s="32"/>
       <c r="Q31" s="33"/>
       <c r="R31" s="33"/>
@@ -9166,53 +9124,53 @@
       </c>
       <c r="AD31" s="21"/>
       <c r="AE31" s="19"/>
-      <c r="AF31" s="112"/>
-      <c r="AG31" s="90"/>
-      <c r="AH31" s="84"/>
-      <c r="AI31" s="84"/>
-      <c r="AJ31" s="84"/>
-      <c r="AK31" s="53"/>
-      <c r="AL31" s="54"/>
-      <c r="AM31" s="147"/>
-      <c r="AN31" s="148"/>
+      <c r="AF31" s="97"/>
+      <c r="AG31" s="69"/>
+      <c r="AH31" s="70"/>
+      <c r="AI31" s="70"/>
+      <c r="AJ31" s="70"/>
+      <c r="AK31" s="73"/>
+      <c r="AL31" s="74"/>
+      <c r="AM31" s="79"/>
+      <c r="AN31" s="80"/>
       <c r="AO31" s="19"/>
       <c r="AP31" s="3"/>
-      <c r="AS31" s="133" t="s">
+      <c r="AS31" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="AW31" s="133">
+      <c r="AW31" s="51">
         <v>1</v>
       </c>
-      <c r="AX31" s="133">
+      <c r="AX31" s="51">
         <v>1</v>
       </c>
-      <c r="AY31" s="133">
+      <c r="AY31" s="51">
         <v>1</v>
       </c>
-      <c r="AZ31" s="133">
+      <c r="AZ31" s="51">
         <v>1</v>
       </c>
-      <c r="BA31" s="133">
+      <c r="BA31" s="51">
         <v>0</v>
       </c>
-      <c r="BB31" s="133">
+      <c r="BB31" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
-      <c r="C32" s="110"/>
-      <c r="D32" s="132"/>
-      <c r="E32" s="132"/>
-      <c r="F32" s="132"/>
-      <c r="G32" s="132"/>
-      <c r="H32" s="132"/>
-      <c r="I32" s="132"/>
-      <c r="J32" s="132"/>
-      <c r="K32" s="132"/>
-      <c r="L32" s="132"/>
-      <c r="M32" s="132"/>
-      <c r="N32" s="132"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="111"/>
+      <c r="E32" s="111"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="111"/>
+      <c r="H32" s="111"/>
+      <c r="I32" s="111"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="111"/>
+      <c r="M32" s="111"/>
+      <c r="N32" s="111"/>
       <c r="O32" s="10"/>
       <c r="P32" s="37"/>
       <c r="Q32" s="10"/>
@@ -9230,368 +9188,368 @@
       <c r="AC32" s="10"/>
       <c r="AD32" s="21"/>
       <c r="AE32" s="19"/>
-      <c r="AF32" s="112"/>
-      <c r="AG32" s="90"/>
-      <c r="AH32" s="84"/>
-      <c r="AI32" s="84"/>
-      <c r="AJ32" s="84"/>
-      <c r="AK32" s="55"/>
-      <c r="AL32" s="56"/>
-      <c r="AM32" s="147"/>
-      <c r="AN32" s="148"/>
+      <c r="AF32" s="97"/>
+      <c r="AG32" s="69"/>
+      <c r="AH32" s="70"/>
+      <c r="AI32" s="70"/>
+      <c r="AJ32" s="70"/>
+      <c r="AK32" s="75"/>
+      <c r="AL32" s="76"/>
+      <c r="AM32" s="79"/>
+      <c r="AN32" s="80"/>
       <c r="AO32" s="19"/>
       <c r="AP32" s="3"/>
-      <c r="AS32" s="133" t="s">
+      <c r="AS32" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="AW32" s="133">
+      <c r="AW32" s="51">
         <v>70.115384615384613</v>
       </c>
-      <c r="AX32" s="133">
+      <c r="AX32" s="51">
         <v>70.115384615384613</v>
       </c>
-      <c r="AY32" s="133">
+      <c r="AY32" s="51">
         <v>70.043478260869563</v>
       </c>
-      <c r="AZ32" s="133">
+      <c r="AZ32" s="51">
         <v>58.086956521739133</v>
       </c>
-      <c r="BA32" s="133">
+      <c r="BA32" s="51">
         <v>101.07142857142857</v>
       </c>
-      <c r="BB32" s="133">
+      <c r="BB32" s="51">
         <v>72.954545454545453</v>
       </c>
     </row>
     <row r="33" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="132"/>
-      <c r="F33" s="132"/>
-      <c r="G33" s="132"/>
-      <c r="H33" s="132"/>
-      <c r="I33" s="132"/>
-      <c r="J33" s="132"/>
-      <c r="K33" s="132"/>
-      <c r="L33" s="132"/>
-      <c r="M33" s="132"/>
-      <c r="N33" s="132"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="111"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="111"/>
+      <c r="I33" s="111"/>
+      <c r="J33" s="111"/>
+      <c r="K33" s="111"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="111"/>
+      <c r="N33" s="111"/>
       <c r="P33" s="39"/>
       <c r="AA33" s="40"/>
       <c r="AD33" s="21"/>
       <c r="AE33" s="19"/>
-      <c r="AF33" s="112"/>
-      <c r="AG33" s="107" t="s">
+      <c r="AF33" s="97"/>
+      <c r="AG33" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="AH33" s="72"/>
-      <c r="AI33" s="72"/>
-      <c r="AJ33" s="72"/>
-      <c r="AK33" s="72"/>
-      <c r="AL33" s="72"/>
-      <c r="AM33" s="72"/>
-      <c r="AN33" s="73"/>
+      <c r="AH33" s="62"/>
+      <c r="AI33" s="62"/>
+      <c r="AJ33" s="62"/>
+      <c r="AK33" s="62"/>
+      <c r="AL33" s="62"/>
+      <c r="AM33" s="62"/>
+      <c r="AN33" s="63"/>
       <c r="AO33" s="19"/>
       <c r="AP33" s="3"/>
-      <c r="AS33" s="133" t="s">
+      <c r="AS33" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="AW33" s="133">
+      <c r="AW33" s="51">
         <v>5</v>
       </c>
-      <c r="AX33" s="133">
+      <c r="AX33" s="51">
         <v>5</v>
       </c>
-      <c r="AY33" s="133">
+      <c r="AY33" s="51">
         <v>3</v>
       </c>
-      <c r="AZ33" s="133">
+      <c r="AZ33" s="51">
         <v>7</v>
       </c>
-      <c r="BA33" s="133">
+      <c r="BA33" s="51">
         <v>7</v>
       </c>
-      <c r="BB33" s="133">
+      <c r="BB33" s="51">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
-      <c r="C34" s="110"/>
-      <c r="D34" s="132"/>
-      <c r="E34" s="132"/>
-      <c r="F34" s="132"/>
-      <c r="G34" s="132"/>
-      <c r="H34" s="132"/>
-      <c r="I34" s="132"/>
-      <c r="J34" s="132"/>
-      <c r="K34" s="132"/>
-      <c r="L34" s="132"/>
-      <c r="M34" s="132"/>
-      <c r="N34" s="132"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="111"/>
+      <c r="F34" s="111"/>
+      <c r="G34" s="111"/>
+      <c r="H34" s="111"/>
+      <c r="I34" s="111"/>
+      <c r="J34" s="111"/>
+      <c r="K34" s="111"/>
+      <c r="L34" s="111"/>
+      <c r="M34" s="111"/>
+      <c r="N34" s="111"/>
       <c r="P34" s="39"/>
       <c r="AA34" s="40"/>
       <c r="AD34" s="21"/>
       <c r="AE34" s="19"/>
-      <c r="AF34" s="112"/>
-      <c r="AG34" s="108"/>
-      <c r="AH34" s="74"/>
-      <c r="AI34" s="74"/>
-      <c r="AJ34" s="74"/>
-      <c r="AK34" s="74"/>
-      <c r="AL34" s="74"/>
-      <c r="AM34" s="74"/>
-      <c r="AN34" s="75"/>
+      <c r="AF34" s="97"/>
+      <c r="AG34" s="64"/>
+      <c r="AH34" s="65"/>
+      <c r="AI34" s="65"/>
+      <c r="AJ34" s="65"/>
+      <c r="AK34" s="65"/>
+      <c r="AL34" s="65"/>
+      <c r="AM34" s="65"/>
+      <c r="AN34" s="66"/>
       <c r="AO34" s="19"/>
       <c r="AP34" s="3"/>
     </row>
     <row r="35" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="132"/>
-      <c r="E35" s="132"/>
-      <c r="F35" s="132"/>
-      <c r="G35" s="132"/>
-      <c r="H35" s="132"/>
-      <c r="I35" s="132"/>
-      <c r="J35" s="132"/>
-      <c r="K35" s="132"/>
-      <c r="L35" s="132"/>
-      <c r="M35" s="132"/>
-      <c r="N35" s="132"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="111"/>
+      <c r="I35" s="111"/>
+      <c r="J35" s="111"/>
+      <c r="K35" s="111"/>
+      <c r="L35" s="111"/>
+      <c r="M35" s="111"/>
+      <c r="N35" s="111"/>
       <c r="P35" s="39"/>
       <c r="AA35" s="40"/>
       <c r="AD35" s="21"/>
       <c r="AE35" s="19"/>
-      <c r="AF35" s="112"/>
+      <c r="AF35" s="97"/>
       <c r="AO35" s="19"/>
       <c r="AP35" s="3"/>
-      <c r="AS35" s="133" t="s">
+      <c r="AS35" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="AW35" s="144">
+      <c r="AW35" s="60">
         <v>1.1395737985651008E-2</v>
       </c>
-      <c r="AX35" s="144">
+      <c r="AX35" s="60">
         <v>1.4073484347259517E-2</v>
       </c>
-      <c r="AY35" s="144">
+      <c r="AY35" s="60">
         <v>1.6490914680101287E-2</v>
       </c>
-      <c r="AZ35" s="144">
+      <c r="AZ35" s="60">
         <v>1.6966455046575634E-2</v>
       </c>
-      <c r="BA35" s="144">
+      <c r="BA35" s="60">
         <v>1.3620751316435028E-2</v>
       </c>
-      <c r="BB35" s="144">
+      <c r="BB35" s="60">
         <v>1.3620751316435028E-2</v>
       </c>
     </row>
     <row r="36" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="132"/>
-      <c r="E36" s="132"/>
-      <c r="F36" s="132"/>
-      <c r="G36" s="132"/>
-      <c r="H36" s="132"/>
-      <c r="I36" s="132"/>
-      <c r="J36" s="132"/>
-      <c r="K36" s="132"/>
-      <c r="L36" s="132"/>
-      <c r="M36" s="132"/>
-      <c r="N36" s="132"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="111"/>
+      <c r="E36" s="111"/>
+      <c r="F36" s="111"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="111"/>
+      <c r="I36" s="111"/>
+      <c r="J36" s="111"/>
+      <c r="K36" s="111"/>
+      <c r="L36" s="111"/>
+      <c r="M36" s="111"/>
+      <c r="N36" s="111"/>
       <c r="P36" s="39"/>
       <c r="AA36" s="40"/>
       <c r="AD36" s="21"/>
       <c r="AE36" s="19"/>
-      <c r="AF36" s="112"/>
-      <c r="AG36" s="102" t="s">
+      <c r="AF36" s="97"/>
+      <c r="AG36" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="AH36" s="83"/>
-      <c r="AI36" s="83"/>
-      <c r="AJ36" s="83"/>
-      <c r="AK36" s="51"/>
-      <c r="AL36" s="52"/>
-      <c r="AM36" s="145">
+      <c r="AH36" s="68"/>
+      <c r="AI36" s="68"/>
+      <c r="AJ36" s="68"/>
+      <c r="AK36" s="71"/>
+      <c r="AL36" s="72"/>
+      <c r="AM36" s="77">
         <v>0</v>
       </c>
-      <c r="AN36" s="146"/>
+      <c r="AN36" s="78"/>
       <c r="AO36" s="19"/>
       <c r="AP36" s="3"/>
     </row>
     <row r="37" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
-      <c r="C37" s="110"/>
-      <c r="D37" s="132"/>
-      <c r="E37" s="132"/>
-      <c r="F37" s="132"/>
-      <c r="G37" s="132"/>
-      <c r="H37" s="132"/>
-      <c r="I37" s="132"/>
-      <c r="J37" s="132"/>
-      <c r="K37" s="132"/>
-      <c r="L37" s="132"/>
-      <c r="M37" s="132"/>
-      <c r="N37" s="132"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="111"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="111"/>
+      <c r="I37" s="111"/>
+      <c r="J37" s="111"/>
+      <c r="K37" s="111"/>
+      <c r="L37" s="111"/>
+      <c r="M37" s="111"/>
+      <c r="N37" s="111"/>
       <c r="P37" s="39"/>
       <c r="AA37" s="40"/>
       <c r="AD37" s="21"/>
       <c r="AE37" s="19"/>
-      <c r="AF37" s="112"/>
-      <c r="AG37" s="90"/>
-      <c r="AH37" s="84"/>
-      <c r="AI37" s="84"/>
-      <c r="AJ37" s="84"/>
-      <c r="AK37" s="53"/>
-      <c r="AL37" s="54"/>
-      <c r="AM37" s="147"/>
-      <c r="AN37" s="148"/>
+      <c r="AF37" s="97"/>
+      <c r="AG37" s="69"/>
+      <c r="AH37" s="70"/>
+      <c r="AI37" s="70"/>
+      <c r="AJ37" s="70"/>
+      <c r="AK37" s="73"/>
+      <c r="AL37" s="74"/>
+      <c r="AM37" s="79"/>
+      <c r="AN37" s="80"/>
       <c r="AO37" s="19"/>
       <c r="AP37" s="3"/>
-      <c r="AS37" s="133" t="s">
+      <c r="AS37" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="AW37" s="133">
+      <c r="AW37" s="51">
         <v>31.875</v>
       </c>
-      <c r="AX37" s="133">
+      <c r="AX37" s="51">
         <v>31.875</v>
       </c>
-      <c r="AY37" s="133">
+      <c r="AY37" s="51">
         <v>35.75</v>
       </c>
-      <c r="AZ37" s="133">
+      <c r="AZ37" s="51">
         <v>36</v>
       </c>
-      <c r="BA37" s="133">
+      <c r="BA37" s="51">
         <v>137.6</v>
       </c>
-      <c r="BB37" s="133">
+      <c r="BB37" s="51">
         <v>137.6</v>
       </c>
     </row>
     <row r="38" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
-      <c r="C38" s="110"/>
-      <c r="D38" s="132"/>
-      <c r="E38" s="132"/>
-      <c r="F38" s="132"/>
-      <c r="G38" s="132"/>
-      <c r="H38" s="132"/>
-      <c r="I38" s="132"/>
-      <c r="J38" s="132"/>
-      <c r="K38" s="132"/>
-      <c r="L38" s="132"/>
-      <c r="M38" s="132"/>
-      <c r="N38" s="132"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="111"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="111"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="111"/>
+      <c r="N38" s="111"/>
       <c r="P38" s="39"/>
       <c r="AA38" s="40"/>
       <c r="AD38" s="21"/>
       <c r="AE38" s="19"/>
-      <c r="AF38" s="112"/>
-      <c r="AG38" s="90"/>
-      <c r="AH38" s="84"/>
-      <c r="AI38" s="84"/>
-      <c r="AJ38" s="84"/>
-      <c r="AK38" s="55"/>
-      <c r="AL38" s="56"/>
-      <c r="AM38" s="147"/>
-      <c r="AN38" s="148"/>
+      <c r="AF38" s="97"/>
+      <c r="AG38" s="69"/>
+      <c r="AH38" s="70"/>
+      <c r="AI38" s="70"/>
+      <c r="AJ38" s="70"/>
+      <c r="AK38" s="75"/>
+      <c r="AL38" s="76"/>
+      <c r="AM38" s="79"/>
+      <c r="AN38" s="80"/>
       <c r="AO38" s="19"/>
       <c r="AP38" s="3"/>
-      <c r="AS38" s="133" t="s">
+      <c r="AS38" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="AW38" s="133">
+      <c r="AW38" s="51">
         <v>3.1468531468531472E-2</v>
       </c>
-      <c r="AX38" s="133">
+      <c r="AX38" s="51">
         <v>2.972027972027972E-2</v>
       </c>
-      <c r="AY38" s="133">
+      <c r="AY38" s="51">
         <v>1.232394366197183E-2</v>
       </c>
-      <c r="AZ38" s="133">
+      <c r="AZ38" s="51">
         <v>1.7605633802816902E-2</v>
       </c>
-      <c r="BA38" s="133">
+      <c r="BA38" s="51">
         <v>1.4388489208633094E-2</v>
       </c>
-      <c r="BB38" s="133">
+      <c r="BB38" s="51">
         <v>1.048951048951049E-2</v>
       </c>
     </row>
     <row r="39" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
-      <c r="C39" s="110"/>
-      <c r="D39" s="132"/>
-      <c r="E39" s="132"/>
-      <c r="F39" s="132"/>
-      <c r="G39" s="132"/>
-      <c r="H39" s="132"/>
-      <c r="I39" s="132"/>
-      <c r="J39" s="132"/>
-      <c r="K39" s="132"/>
-      <c r="L39" s="132"/>
-      <c r="M39" s="132"/>
-      <c r="N39" s="132"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="111"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="111"/>
+      <c r="G39" s="111"/>
+      <c r="H39" s="111"/>
+      <c r="I39" s="111"/>
+      <c r="J39" s="111"/>
+      <c r="K39" s="111"/>
+      <c r="L39" s="111"/>
+      <c r="M39" s="111"/>
+      <c r="N39" s="111"/>
       <c r="P39" s="39"/>
       <c r="AA39" s="40"/>
       <c r="AD39" s="21"/>
       <c r="AE39" s="19"/>
-      <c r="AF39" s="112"/>
-      <c r="AG39" s="107" t="s">
+      <c r="AF39" s="97"/>
+      <c r="AG39" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="AH39" s="72"/>
-      <c r="AI39" s="72"/>
-      <c r="AJ39" s="72"/>
-      <c r="AK39" s="72"/>
-      <c r="AL39" s="72"/>
-      <c r="AM39" s="72"/>
-      <c r="AN39" s="73"/>
+      <c r="AH39" s="62"/>
+      <c r="AI39" s="62"/>
+      <c r="AJ39" s="62"/>
+      <c r="AK39" s="62"/>
+      <c r="AL39" s="62"/>
+      <c r="AM39" s="62"/>
+      <c r="AN39" s="63"/>
       <c r="AO39" s="19"/>
       <c r="AP39" s="3"/>
-      <c r="AS39" s="133" t="s">
+      <c r="AS39" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="AW39" s="133">
+      <c r="AW39" s="51">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="AX39" s="133">
+      <c r="AX39" s="51">
         <v>0.2</v>
       </c>
-      <c r="AY39" s="133">
+      <c r="AY39" s="51">
         <v>0.1111111111111111</v>
       </c>
-      <c r="AZ39" s="133">
+      <c r="AZ39" s="51">
         <v>0</v>
       </c>
-      <c r="BA39" s="133">
+      <c r="BA39" s="51">
         <v>0</v>
       </c>
-      <c r="BB39" s="133">
+      <c r="BB39" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
-      <c r="C40" s="110"/>
-      <c r="D40" s="132"/>
-      <c r="E40" s="132"/>
-      <c r="F40" s="132"/>
-      <c r="G40" s="132"/>
-      <c r="H40" s="132"/>
-      <c r="I40" s="132"/>
-      <c r="J40" s="132"/>
-      <c r="K40" s="132"/>
-      <c r="L40" s="132"/>
-      <c r="M40" s="132"/>
-      <c r="N40" s="132"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="111"/>
+      <c r="I40" s="111"/>
+      <c r="J40" s="111"/>
+      <c r="K40" s="111"/>
+      <c r="L40" s="111"/>
+      <c r="M40" s="111"/>
+      <c r="N40" s="111"/>
       <c r="P40" s="41"/>
       <c r="Q40" s="42"/>
       <c r="R40" s="42"/>
@@ -9606,21 +9564,21 @@
       <c r="AA40" s="43"/>
       <c r="AD40" s="21"/>
       <c r="AE40" s="19"/>
-      <c r="AF40" s="112"/>
-      <c r="AG40" s="108"/>
-      <c r="AH40" s="74"/>
-      <c r="AI40" s="74"/>
-      <c r="AJ40" s="74"/>
-      <c r="AK40" s="74"/>
-      <c r="AL40" s="74"/>
-      <c r="AM40" s="74"/>
-      <c r="AN40" s="75"/>
+      <c r="AF40" s="97"/>
+      <c r="AG40" s="64"/>
+      <c r="AH40" s="65"/>
+      <c r="AI40" s="65"/>
+      <c r="AJ40" s="65"/>
+      <c r="AK40" s="65"/>
+      <c r="AL40" s="65"/>
+      <c r="AM40" s="65"/>
+      <c r="AN40" s="66"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="3"/>
     </row>
     <row r="41" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
-      <c r="C41" s="111"/>
+      <c r="C41" s="96"/>
       <c r="D41" s="44"/>
       <c r="E41" s="44"/>
       <c r="F41" s="44"/>
@@ -9649,7 +9607,7 @@
       <c r="AC41" s="44"/>
       <c r="AD41" s="45"/>
       <c r="AE41" s="19"/>
-      <c r="AF41" s="113"/>
+      <c r="AF41" s="98"/>
       <c r="AG41" s="16"/>
       <c r="AH41" s="16"/>
       <c r="AI41" s="16"/>
@@ -9660,34 +9618,34 @@
       <c r="AN41" s="16"/>
       <c r="AO41" s="46"/>
       <c r="AP41" s="3"/>
-      <c r="AS41" s="133" t="s">
+      <c r="AS41" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="AW41" s="144">
+      <c r="AW41" s="60">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="AX41" s="144">
+      <c r="AX41" s="60">
         <v>0.2673611111111111</v>
       </c>
-      <c r="AY41" s="144">
+      <c r="AY41" s="60">
         <v>0.125</v>
       </c>
-      <c r="AZ41" s="144">
+      <c r="AZ41" s="60">
         <v>0.36458333333333331</v>
       </c>
-      <c r="BA41" s="144">
+      <c r="BA41" s="60">
         <v>0.5</v>
       </c>
-      <c r="BB41" s="144">
+      <c r="BB41" s="60">
         <v>0.5</v>
       </c>
-      <c r="BD41" s="133" t="s">
+      <c r="BD41" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="BE41" s="133" t="s">
+      <c r="BE41" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="BF41" s="133" t="s">
+      <c r="BF41" s="51" t="s">
         <v>66</v>
       </c>
     </row>
@@ -9733,18 +9691,18 @@
       <c r="AN42" s="48"/>
       <c r="AO42" s="48"/>
       <c r="AP42" s="49"/>
-      <c r="AS42" s="133" t="s">
+      <c r="AS42" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="BB42" s="133">
+      <c r="BB42" s="51">
         <v>853200</v>
       </c>
     </row>
     <row r="43" spans="2:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AS43" s="133" t="s">
+      <c r="AS43" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="BB43" s="133">
+      <c r="BB43" s="51">
         <v>2.1</v>
       </c>
     </row>
@@ -9769,23 +9727,59 @@
       <c r="AL51" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="auPPL+J0ZZCyowdRDEV8btVzK5cz2iJhuVEEIsj7qJWE7id3ihEVtUqLstvZAcUoIkoxQr07hn/yQ3Dqk0Dtaw==" saltValue="dENWaYPdoxJgl6b/6X54DQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="83">
-    <mergeCell ref="AG39:AN40"/>
-    <mergeCell ref="AG30:AJ32"/>
-    <mergeCell ref="AK30:AL32"/>
-    <mergeCell ref="AM30:AN32"/>
-    <mergeCell ref="AG33:AN34"/>
-    <mergeCell ref="AG36:AJ38"/>
-    <mergeCell ref="AK36:AL38"/>
-    <mergeCell ref="AM36:AN38"/>
-    <mergeCell ref="AG24:AJ26"/>
-    <mergeCell ref="AK24:AL26"/>
-    <mergeCell ref="AM24:AN26"/>
-    <mergeCell ref="O27:R28"/>
-    <mergeCell ref="V27:AC28"/>
-    <mergeCell ref="AG27:AN28"/>
-    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="AW2:AW4"/>
+    <mergeCell ref="AX2:AX4"/>
+    <mergeCell ref="AB5:AC7"/>
+    <mergeCell ref="B2:AP3"/>
+    <mergeCell ref="AT2:AT4"/>
+    <mergeCell ref="AU2:AU4"/>
+    <mergeCell ref="AV2:AV4"/>
+    <mergeCell ref="AM10:AN12"/>
+    <mergeCell ref="AD5:AE7"/>
+    <mergeCell ref="AF5:AN7"/>
+    <mergeCell ref="C9:C21"/>
+    <mergeCell ref="W9:W21"/>
+    <mergeCell ref="D10:G12"/>
+    <mergeCell ref="H10:I12"/>
+    <mergeCell ref="J10:K12"/>
+    <mergeCell ref="M10:P12"/>
+    <mergeCell ref="Q10:R12"/>
+    <mergeCell ref="S10:T12"/>
+    <mergeCell ref="D5:G7"/>
+    <mergeCell ref="H5:I7"/>
+    <mergeCell ref="J5:K7"/>
+    <mergeCell ref="L5:T7"/>
+    <mergeCell ref="X5:AA7"/>
+    <mergeCell ref="X10:AA12"/>
+    <mergeCell ref="AB10:AC12"/>
+    <mergeCell ref="AD10:AE12"/>
+    <mergeCell ref="AG10:AJ12"/>
+    <mergeCell ref="AK10:AL12"/>
+    <mergeCell ref="D13:K14"/>
+    <mergeCell ref="M13:T14"/>
+    <mergeCell ref="X13:AE14"/>
+    <mergeCell ref="AG13:AN14"/>
+    <mergeCell ref="D16:G18"/>
+    <mergeCell ref="H16:I18"/>
+    <mergeCell ref="J16:K18"/>
+    <mergeCell ref="M16:P18"/>
+    <mergeCell ref="Q16:R18"/>
+    <mergeCell ref="S16:T18"/>
+    <mergeCell ref="AY15:AY17"/>
+    <mergeCell ref="X16:AA18"/>
+    <mergeCell ref="AB16:AC18"/>
+    <mergeCell ref="AD16:AE18"/>
+    <mergeCell ref="AG16:AJ18"/>
+    <mergeCell ref="AK16:AL18"/>
+    <mergeCell ref="AM16:AN18"/>
+    <mergeCell ref="C23:C41"/>
+    <mergeCell ref="AF23:AF41"/>
+    <mergeCell ref="O24:R26"/>
+    <mergeCell ref="V24:Y26"/>
+    <mergeCell ref="Z24:AA26"/>
+    <mergeCell ref="AB24:AC26"/>
+    <mergeCell ref="D24:N40"/>
     <mergeCell ref="BF15:BF17"/>
     <mergeCell ref="D19:K20"/>
     <mergeCell ref="M19:T20"/>
@@ -9802,78 +9796,217 @@
     <mergeCell ref="AV15:AV17"/>
     <mergeCell ref="AW15:AW17"/>
     <mergeCell ref="AX15:AX17"/>
-    <mergeCell ref="C23:C41"/>
-    <mergeCell ref="AF23:AF41"/>
-    <mergeCell ref="O24:R26"/>
-    <mergeCell ref="V24:Y26"/>
-    <mergeCell ref="Z24:AA26"/>
-    <mergeCell ref="AB24:AC26"/>
-    <mergeCell ref="D24:N40"/>
-    <mergeCell ref="AY15:AY17"/>
-    <mergeCell ref="X16:AA18"/>
-    <mergeCell ref="AB16:AC18"/>
-    <mergeCell ref="AD16:AE18"/>
-    <mergeCell ref="AG16:AJ18"/>
-    <mergeCell ref="AK16:AL18"/>
-    <mergeCell ref="AM16:AN18"/>
-    <mergeCell ref="D13:K14"/>
-    <mergeCell ref="M13:T14"/>
-    <mergeCell ref="X13:AE14"/>
-    <mergeCell ref="AG13:AN14"/>
-    <mergeCell ref="D16:G18"/>
-    <mergeCell ref="H16:I18"/>
-    <mergeCell ref="J16:K18"/>
-    <mergeCell ref="M16:P18"/>
-    <mergeCell ref="Q16:R18"/>
-    <mergeCell ref="S16:T18"/>
-    <mergeCell ref="X10:AA12"/>
-    <mergeCell ref="AB10:AC12"/>
-    <mergeCell ref="AD10:AE12"/>
-    <mergeCell ref="AG10:AJ12"/>
-    <mergeCell ref="AK10:AL12"/>
-    <mergeCell ref="AM10:AN12"/>
-    <mergeCell ref="AD5:AE7"/>
-    <mergeCell ref="AF5:AN7"/>
-    <mergeCell ref="C9:C21"/>
-    <mergeCell ref="W9:W21"/>
-    <mergeCell ref="D10:G12"/>
-    <mergeCell ref="H10:I12"/>
-    <mergeCell ref="J10:K12"/>
-    <mergeCell ref="M10:P12"/>
-    <mergeCell ref="Q10:R12"/>
-    <mergeCell ref="S10:T12"/>
-    <mergeCell ref="D5:G7"/>
-    <mergeCell ref="H5:I7"/>
-    <mergeCell ref="J5:K7"/>
-    <mergeCell ref="L5:T7"/>
-    <mergeCell ref="X5:AA7"/>
-    <mergeCell ref="AW2:AW4"/>
-    <mergeCell ref="AX2:AX4"/>
-    <mergeCell ref="AB5:AC7"/>
-    <mergeCell ref="B2:AP3"/>
-    <mergeCell ref="AT2:AT4"/>
-    <mergeCell ref="AU2:AU4"/>
-    <mergeCell ref="AV2:AV4"/>
+    <mergeCell ref="AG24:AJ26"/>
+    <mergeCell ref="AK24:AL26"/>
+    <mergeCell ref="AM24:AN26"/>
+    <mergeCell ref="O27:R28"/>
+    <mergeCell ref="V27:AC28"/>
+    <mergeCell ref="AG27:AN28"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="AG39:AN40"/>
+    <mergeCell ref="AG30:AJ32"/>
+    <mergeCell ref="AK30:AL32"/>
+    <mergeCell ref="AM30:AN32"/>
+    <mergeCell ref="AG33:AN34"/>
+    <mergeCell ref="AG36:AJ38"/>
+    <mergeCell ref="AK36:AL38"/>
+    <mergeCell ref="AM36:AN38"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="36" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup manualMax="1" manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" maxAxisType="custom" xr2:uid="{F4C40EA9-3578-924E-BF1B-802D85E6C5CE}">
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{C52E2EB6-BD76-1645-838C-EA4ABC745F92}">
           <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
           <x14:colorMarkers rgb="FFD00000"/>
           <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast theme="0" tint="-0.249977111117893"/>
+          <x14:colorLast rgb="FF00B050"/>
           <x14:colorHigh rgb="FFD00000"/>
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Team Metrics'!AW22:BB22</xm:f>
-              <xm:sqref>H5</xm:sqref>
+              <xm:f>'Team Metrics'!AW39:BB39</xm:f>
+              <xm:sqref>AK36</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMax="5.000000000000001E-2" manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" maxAxisType="custom" xr2:uid="{08A56B59-F19C-3B49-AA94-3E18910DA689}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FF00B050"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW38:BB38</xm:f>
+              <xm:sqref>AK30</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{FB7F1646-3097-0544-B21B-D763618232EC}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FF339966"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW37:BB37</xm:f>
+              <xm:sqref>AK24</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{2DFB55D3-4B11-F440-BFAC-22DA08EF9038}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFFFC000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW35:BB35</xm:f>
+              <xm:sqref>Z24</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{A5168FF9-78DB-8248-9AAF-8FE3FB223891}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFCC3399"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW33:BB33</xm:f>
+              <xm:sqref>AK16</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{93FA3AA0-7E52-E149-A6D5-ECD37C015879}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFCC3399"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW32:BB32</xm:f>
+              <xm:sqref>AB16</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{F1505BFD-1AD4-FB47-AE32-37CCBD8D61C0}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFCC3399"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW31:BB31</xm:f>
+              <xm:sqref>AK10</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{A0F97C6B-D297-B74F-A0BD-1A05372E32AD}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFCC3399"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW30:BB30</xm:f>
+              <xm:sqref>AB10</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{5D70A36A-8281-9E4B-ACB6-1E8652E5AEAE}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FF4472C4"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW28:BB28</xm:f>
+              <xm:sqref>Q16</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{E2C88339-FCB1-2041-BF1A-EF6E8F9A95A0}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FF4472C4"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW27:BB27</xm:f>
+              <xm:sqref>H16</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{7A4F7879-1C4B-3C4A-A294-1973EC8C5D8E}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FF4472C4"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW26:BB26</xm:f>
+              <xm:sqref>Q10</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{38E95271-B073-1E48-BFC5-66D15BDE9BB0}">
+          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FF4472C4"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Team Metrics'!AW25:BB25</xm:f>
+              <xm:sqref>H10</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -9893,195 +10026,19 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{38E95271-B073-1E48-BFC5-66D15BDE9BB0}">
+        <x14:sparklineGroup manualMax="1" manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" maxAxisType="custom" xr2:uid="{F4C40EA9-3578-924E-BF1B-802D85E6C5CE}">
           <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
           <x14:colorMarkers rgb="FFD00000"/>
           <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FF4472C4"/>
+          <x14:colorLast theme="0" tint="-0.249977111117893"/>
           <x14:colorHigh rgb="FFD00000"/>
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Team Metrics'!AW25:BB25</xm:f>
-              <xm:sqref>H10</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{7A4F7879-1C4B-3C4A-A294-1973EC8C5D8E}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FF4472C4"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW26:BB26</xm:f>
-              <xm:sqref>Q10</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{E2C88339-FCB1-2041-BF1A-EF6E8F9A95A0}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FF4472C4"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW27:BB27</xm:f>
-              <xm:sqref>H16</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{5D70A36A-8281-9E4B-ACB6-1E8652E5AEAE}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FF4472C4"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW28:BB28</xm:f>
-              <xm:sqref>Q16</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{A0F97C6B-D297-B74F-A0BD-1A05372E32AD}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFCC3399"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW30:BB30</xm:f>
-              <xm:sqref>AB10</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{F1505BFD-1AD4-FB47-AE32-37CCBD8D61C0}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFCC3399"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW31:BB31</xm:f>
-              <xm:sqref>AK10</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{93FA3AA0-7E52-E149-A6D5-ECD37C015879}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFCC3399"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW32:BB32</xm:f>
-              <xm:sqref>AB16</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{A5168FF9-78DB-8248-9AAF-8FE3FB223891}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFCC3399"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW33:BB33</xm:f>
-              <xm:sqref>AK16</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{2DFB55D3-4B11-F440-BFAC-22DA08EF9038}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFFFC000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW35:BB35</xm:f>
-              <xm:sqref>Z24</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{FB7F1646-3097-0544-B21B-D763618232EC}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FF339966"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW37:BB37</xm:f>
-              <xm:sqref>AK24</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="5.000000000000001E-2" manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" maxAxisType="custom" xr2:uid="{08A56B59-F19C-3B49-AA94-3E18910DA689}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FF00B050"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW38:BB38</xm:f>
-              <xm:sqref>AK30</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup manualMin="0" type="column" displayEmptyCellsAs="gap" last="1" minAxisType="custom" xr2:uid="{C52E2EB6-BD76-1645-838C-EA4ABC745F92}">
-          <x14:colorSeries theme="0" tint="-4.9989318521683403E-2"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FF00B050"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Team Metrics'!AW39:BB39</xm:f>
-              <xm:sqref>AK36</xm:sqref>
+              <xm:f>'Team Metrics'!AW22:BB22</xm:f>
+              <xm:sqref>H5</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>